<commit_message>
Vari bug, drop colonne, merge wellness
fixato bug su giorni di gara(probabilmente)
drop di colonne di dati brutti, comunque fatto in chiaro e modificabile facilmente
mergato il file di wellness
</commit_message>
<xml_diff>
--- a/Datasets/sessioni_workload.xlsx
+++ b/Datasets/sessioni_workload.xlsx
@@ -12955,12 +12955,24 @@
       <c r="B261" t="s">
         <v>194</v>
       </c>
-      <c r="C261" t="s"/>
-      <c r="D261" t="s"/>
-      <c r="E261" t="s"/>
-      <c r="F261" t="s"/>
-      <c r="G261" t="s"/>
-      <c r="H261" t="s"/>
+      <c r="C261" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="D261" t="n">
+        <v>65.7</v>
+      </c>
+      <c r="E261" t="n">
+        <v>60.7</v>
+      </c>
+      <c r="F261" t="n">
+        <v>80.2</v>
+      </c>
+      <c r="G261" t="n">
+        <v>74.7</v>
+      </c>
+      <c r="H261" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="262" spans="1:8">
       <c r="A262" s="1" t="n">
@@ -12969,12 +12981,24 @@
       <c r="B262" t="s">
         <v>195</v>
       </c>
-      <c r="C262" t="s"/>
-      <c r="D262" t="s"/>
-      <c r="E262" t="s"/>
-      <c r="F262" t="s"/>
-      <c r="G262" t="s"/>
-      <c r="H262" t="s"/>
+      <c r="C262" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="D262" t="n">
+        <v>73.90000000000001</v>
+      </c>
+      <c r="E262" t="n">
+        <v>75.40000000000001</v>
+      </c>
+      <c r="F262" t="n">
+        <v>67.5</v>
+      </c>
+      <c r="G262" t="n">
+        <v>68.8</v>
+      </c>
+      <c r="H262" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="263" spans="1:8">
       <c r="A263" s="1" t="n">
@@ -13009,12 +13033,24 @@
       <c r="B264" t="s">
         <v>197</v>
       </c>
-      <c r="C264" t="s"/>
-      <c r="D264" t="s"/>
-      <c r="E264" t="s"/>
-      <c r="F264" t="s"/>
-      <c r="G264" t="s"/>
-      <c r="H264" t="s"/>
+      <c r="C264" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="D264" t="n">
+        <v>66.59999999999999</v>
+      </c>
+      <c r="E264" t="n">
+        <v>51.7</v>
+      </c>
+      <c r="F264" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="G264" t="n">
+        <v>54.7</v>
+      </c>
+      <c r="H264" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="265" spans="1:8">
       <c r="A265" s="1" t="n">
@@ -13101,12 +13137,24 @@
       <c r="B268" t="s">
         <v>197</v>
       </c>
-      <c r="C268" t="s"/>
-      <c r="D268" t="s"/>
-      <c r="E268" t="s"/>
-      <c r="F268" t="s"/>
-      <c r="G268" t="s"/>
-      <c r="H268" t="s"/>
+      <c r="C268" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="D268" t="n">
+        <v>63.4</v>
+      </c>
+      <c r="E268" t="n">
+        <v>59.3</v>
+      </c>
+      <c r="F268" t="n">
+        <v>54.3</v>
+      </c>
+      <c r="G268" t="n">
+        <v>53.8</v>
+      </c>
+      <c r="H268" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="269" spans="1:8">
       <c r="A269" s="1" t="n">
@@ -13115,12 +13163,24 @@
       <c r="B269" t="s">
         <v>200</v>
       </c>
-      <c r="C269" t="s"/>
-      <c r="D269" t="s"/>
-      <c r="E269" t="s"/>
-      <c r="F269" t="s"/>
-      <c r="G269" t="s"/>
-      <c r="H269" t="s"/>
+      <c r="C269" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="D269" t="n">
+        <v>73.09999999999999</v>
+      </c>
+      <c r="E269" t="n">
+        <v>48.9</v>
+      </c>
+      <c r="F269" t="n">
+        <v>48.7</v>
+      </c>
+      <c r="G269" t="n">
+        <v>55.8</v>
+      </c>
+      <c r="H269" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="270" spans="1:8">
       <c r="A270" s="1" t="n">
@@ -13129,12 +13189,24 @@
       <c r="B270" t="s">
         <v>201</v>
       </c>
-      <c r="C270" t="s"/>
-      <c r="D270" t="s"/>
-      <c r="E270" t="s"/>
-      <c r="F270" t="s"/>
-      <c r="G270" t="s"/>
-      <c r="H270" t="s"/>
+      <c r="C270" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="D270" t="n">
+        <v>89.2</v>
+      </c>
+      <c r="E270" t="n">
+        <v>62.6</v>
+      </c>
+      <c r="F270" t="n">
+        <v>80.09999999999999</v>
+      </c>
+      <c r="G270" t="n">
+        <v>58.1</v>
+      </c>
+      <c r="H270" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="271" spans="1:8">
       <c r="A271" s="1" t="n">
@@ -13195,12 +13267,24 @@
       <c r="B273" t="s">
         <v>200</v>
       </c>
-      <c r="C273" t="s"/>
-      <c r="D273" t="s"/>
-      <c r="E273" t="s"/>
-      <c r="F273" t="s"/>
-      <c r="G273" t="s"/>
-      <c r="H273" t="s"/>
+      <c r="C273" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="D273" t="n">
+        <v>95.09999999999999</v>
+      </c>
+      <c r="E273" t="n">
+        <v>71</v>
+      </c>
+      <c r="F273" t="n">
+        <v>82.59999999999999</v>
+      </c>
+      <c r="G273" t="n">
+        <v>77.2</v>
+      </c>
+      <c r="H273" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="274" spans="1:8">
       <c r="A274" s="1" t="n">
@@ -14507,12 +14591,24 @@
       <c r="B324" t="s">
         <v>197</v>
       </c>
-      <c r="C324" t="s"/>
-      <c r="D324" t="s"/>
-      <c r="E324" t="s"/>
-      <c r="F324" t="s"/>
-      <c r="G324" t="s"/>
-      <c r="H324" t="s"/>
+      <c r="C324" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="D324" t="n">
+        <v>76</v>
+      </c>
+      <c r="E324" t="n">
+        <v>56.4</v>
+      </c>
+      <c r="F324" t="n">
+        <v>61.7</v>
+      </c>
+      <c r="G324" t="n">
+        <v>70.40000000000001</v>
+      </c>
+      <c r="H324" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="325" spans="1:8">
       <c r="A325" s="1" t="n">
@@ -14521,12 +14617,24 @@
       <c r="B325" t="s">
         <v>195</v>
       </c>
-      <c r="C325" t="s"/>
-      <c r="D325" t="s"/>
-      <c r="E325" t="s"/>
-      <c r="F325" t="s"/>
-      <c r="G325" t="s"/>
-      <c r="H325" t="s"/>
+      <c r="C325" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="D325" t="n">
+        <v>97.59999999999999</v>
+      </c>
+      <c r="E325" t="n">
+        <v>106.1</v>
+      </c>
+      <c r="F325" t="n">
+        <v>90.7</v>
+      </c>
+      <c r="G325" t="n">
+        <v>96</v>
+      </c>
+      <c r="H325" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="326" spans="1:8">
       <c r="A326" s="1" t="n">
@@ -14561,12 +14669,24 @@
       <c r="B327" t="s">
         <v>247</v>
       </c>
-      <c r="C327" t="s"/>
-      <c r="D327" t="s"/>
-      <c r="E327" t="s"/>
-      <c r="F327" t="s"/>
-      <c r="G327" t="s"/>
-      <c r="H327" t="s"/>
+      <c r="C327" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="D327" t="n">
+        <v>78.90000000000001</v>
+      </c>
+      <c r="E327" t="n">
+        <v>51.4</v>
+      </c>
+      <c r="F327" t="n">
+        <v>48</v>
+      </c>
+      <c r="G327" t="n">
+        <v>49.6</v>
+      </c>
+      <c r="H327" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="328" spans="1:8">
       <c r="A328" s="1" t="n">
@@ -14627,12 +14747,24 @@
       <c r="B330" t="s">
         <v>197</v>
       </c>
-      <c r="C330" t="s"/>
-      <c r="D330" t="s"/>
-      <c r="E330" t="s"/>
-      <c r="F330" t="s"/>
-      <c r="G330" t="s"/>
-      <c r="H330" t="s"/>
+      <c r="C330" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="D330" t="n">
+        <v>85.40000000000001</v>
+      </c>
+      <c r="E330" t="n">
+        <v>96.59999999999999</v>
+      </c>
+      <c r="F330" t="n">
+        <v>93</v>
+      </c>
+      <c r="G330" t="n">
+        <v>91.90000000000001</v>
+      </c>
+      <c r="H330" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="331" spans="1:8">
       <c r="A331" s="1" t="n">
@@ -14641,12 +14773,24 @@
       <c r="B331" t="s">
         <v>197</v>
       </c>
-      <c r="C331" t="s"/>
-      <c r="D331" t="s"/>
-      <c r="E331" t="s"/>
-      <c r="F331" t="s"/>
-      <c r="G331" t="s"/>
-      <c r="H331" t="s"/>
+      <c r="C331" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="D331" t="n">
+        <v>97.59999999999999</v>
+      </c>
+      <c r="E331" t="n">
+        <v>86.09999999999999</v>
+      </c>
+      <c r="F331" t="n">
+        <v>76.59999999999999</v>
+      </c>
+      <c r="G331" t="n">
+        <v>74.7</v>
+      </c>
+      <c r="H331" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="332" spans="1:8">
       <c r="A332" s="1" t="n">
@@ -14655,12 +14799,24 @@
       <c r="B332" t="s">
         <v>247</v>
       </c>
-      <c r="C332" t="s"/>
-      <c r="D332" t="s"/>
-      <c r="E332" t="s"/>
-      <c r="F332" t="s"/>
-      <c r="G332" t="s"/>
-      <c r="H332" t="s"/>
+      <c r="C332" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="D332" t="n">
+        <v>99.09999999999999</v>
+      </c>
+      <c r="E332" t="n">
+        <v>73.7</v>
+      </c>
+      <c r="F332" t="n">
+        <v>71</v>
+      </c>
+      <c r="G332" t="n">
+        <v>67</v>
+      </c>
+      <c r="H332" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="333" spans="1:8">
       <c r="A333" s="1" t="n">
@@ -14721,12 +14877,24 @@
       <c r="B335" t="s">
         <v>197</v>
       </c>
-      <c r="C335" t="s"/>
-      <c r="D335" t="s"/>
-      <c r="E335" t="s"/>
-      <c r="F335" t="s"/>
-      <c r="G335" t="s"/>
-      <c r="H335" t="s"/>
+      <c r="C335" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="D335" t="n">
+        <v>86.8</v>
+      </c>
+      <c r="E335" t="n">
+        <v>82.2</v>
+      </c>
+      <c r="F335" t="n">
+        <v>68.5</v>
+      </c>
+      <c r="G335" t="n">
+        <v>73.09999999999999</v>
+      </c>
+      <c r="H335" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="336" spans="1:8">
       <c r="A336" s="1" t="n">
@@ -14735,12 +14903,24 @@
       <c r="B336" t="s">
         <v>247</v>
       </c>
-      <c r="C336" t="s"/>
-      <c r="D336" t="s"/>
-      <c r="E336" t="s"/>
-      <c r="F336" t="s"/>
-      <c r="G336" t="s"/>
-      <c r="H336" t="s"/>
+      <c r="C336" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="D336" t="n">
+        <v>73.40000000000001</v>
+      </c>
+      <c r="E336" t="n">
+        <v>71.90000000000001</v>
+      </c>
+      <c r="F336" t="n">
+        <v>81.59999999999999</v>
+      </c>
+      <c r="G336" t="n">
+        <v>54</v>
+      </c>
+      <c r="H336" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="337" spans="1:8">
       <c r="A337" s="1" t="n">
@@ -43441,12 +43621,24 @@
       <c r="B1441" t="s">
         <v>194</v>
       </c>
-      <c r="C1441" t="s"/>
-      <c r="D1441" t="s"/>
-      <c r="E1441" t="s"/>
-      <c r="F1441" t="s"/>
-      <c r="G1441" t="s"/>
-      <c r="H1441" t="s"/>
+      <c r="C1441" t="n">
+        <v>5</v>
+      </c>
+      <c r="D1441" t="n">
+        <v>103.2</v>
+      </c>
+      <c r="E1441" t="n">
+        <v>101.8</v>
+      </c>
+      <c r="F1441" t="n">
+        <v>100</v>
+      </c>
+      <c r="G1441" t="n">
+        <v>94.2</v>
+      </c>
+      <c r="H1441" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="1442" spans="1:8">
       <c r="A1442" s="1" t="n">
@@ -43455,12 +43647,24 @@
       <c r="B1442" t="s">
         <v>247</v>
       </c>
-      <c r="C1442" t="s"/>
-      <c r="D1442" t="s"/>
-      <c r="E1442" t="s"/>
-      <c r="F1442" t="s"/>
-      <c r="G1442" t="s"/>
-      <c r="H1442" t="s"/>
+      <c r="C1442" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="D1442" t="n">
+        <v>67.7</v>
+      </c>
+      <c r="E1442" t="n">
+        <v>82.59999999999999</v>
+      </c>
+      <c r="F1442" t="n">
+        <v>76</v>
+      </c>
+      <c r="G1442" t="n">
+        <v>60.7</v>
+      </c>
+      <c r="H1442" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="1443" spans="1:8">
       <c r="A1443" s="1" t="n">
@@ -43469,12 +43673,24 @@
       <c r="B1443" t="s">
         <v>195</v>
       </c>
-      <c r="C1443" t="s"/>
-      <c r="D1443" t="s"/>
-      <c r="E1443" t="s"/>
-      <c r="F1443" t="s"/>
-      <c r="G1443" t="s"/>
-      <c r="H1443" t="s"/>
+      <c r="C1443" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="D1443" t="n">
+        <v>98</v>
+      </c>
+      <c r="E1443" t="n">
+        <v>90.8</v>
+      </c>
+      <c r="F1443" t="n">
+        <v>84.40000000000001</v>
+      </c>
+      <c r="G1443" t="n">
+        <v>81</v>
+      </c>
+      <c r="H1443" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="1444" spans="1:8">
       <c r="A1444" s="1" t="n">
@@ -43483,12 +43699,24 @@
       <c r="B1444" t="s">
         <v>197</v>
       </c>
-      <c r="C1444" t="s"/>
-      <c r="D1444" t="s"/>
-      <c r="E1444" t="s"/>
-      <c r="F1444" t="s"/>
-      <c r="G1444" t="s"/>
-      <c r="H1444" t="s"/>
+      <c r="C1444" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="D1444" t="n">
+        <v>77.3</v>
+      </c>
+      <c r="E1444" t="n">
+        <v>79.5</v>
+      </c>
+      <c r="F1444" t="n">
+        <v>66.09999999999999</v>
+      </c>
+      <c r="G1444" t="n">
+        <v>86.7</v>
+      </c>
+      <c r="H1444" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="1445" spans="1:8">
       <c r="A1445" s="1" t="n">
@@ -43497,12 +43725,24 @@
       <c r="B1445" t="s">
         <v>247</v>
       </c>
-      <c r="C1445" t="s"/>
-      <c r="D1445" t="s"/>
-      <c r="E1445" t="s"/>
-      <c r="F1445" t="s"/>
-      <c r="G1445" t="s"/>
-      <c r="H1445" t="s"/>
+      <c r="C1445" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="D1445" t="n">
+        <v>89.09999999999999</v>
+      </c>
+      <c r="E1445" t="n">
+        <v>109</v>
+      </c>
+      <c r="F1445" t="n">
+        <v>112.6</v>
+      </c>
+      <c r="G1445" t="n">
+        <v>101.9</v>
+      </c>
+      <c r="H1445" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="1446" spans="1:8">
       <c r="A1446" s="1" t="n">
@@ -43511,12 +43751,24 @@
       <c r="B1446" t="s">
         <v>195</v>
       </c>
-      <c r="C1446" t="s"/>
-      <c r="D1446" t="s"/>
-      <c r="E1446" t="s"/>
-      <c r="F1446" t="s"/>
-      <c r="G1446" t="s"/>
-      <c r="H1446" t="s"/>
+      <c r="C1446" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="D1446" t="n">
+        <v>102.1</v>
+      </c>
+      <c r="E1446" t="n">
+        <v>82.3</v>
+      </c>
+      <c r="F1446" t="n">
+        <v>84.3</v>
+      </c>
+      <c r="G1446" t="n">
+        <v>80.09999999999999</v>
+      </c>
+      <c r="H1446" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="1447" spans="1:8">
       <c r="A1447" s="1" t="n">
@@ -45501,12 +45753,24 @@
       <c r="B1523" t="s">
         <v>247</v>
       </c>
-      <c r="C1523" t="s"/>
-      <c r="D1523" t="s"/>
-      <c r="E1523" t="s"/>
-      <c r="F1523" t="s"/>
-      <c r="G1523" t="s"/>
-      <c r="H1523" t="s"/>
+      <c r="C1523" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="D1523" t="n">
+        <v>94.40000000000001</v>
+      </c>
+      <c r="E1523" t="n">
+        <v>89.59999999999999</v>
+      </c>
+      <c r="F1523" t="n">
+        <v>85.40000000000001</v>
+      </c>
+      <c r="G1523" t="n">
+        <v>84.90000000000001</v>
+      </c>
+      <c r="H1523" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="1524" spans="1:8">
       <c r="A1524" s="1" t="n">
@@ -45515,12 +45779,24 @@
       <c r="B1524" t="s">
         <v>197</v>
       </c>
-      <c r="C1524" t="s"/>
-      <c r="D1524" t="s"/>
-      <c r="E1524" t="s"/>
-      <c r="F1524" t="s"/>
-      <c r="G1524" t="s"/>
-      <c r="H1524" t="s"/>
+      <c r="C1524" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="D1524" t="n">
+        <v>37.9</v>
+      </c>
+      <c r="E1524" t="n">
+        <v>83.7</v>
+      </c>
+      <c r="F1524" t="n">
+        <v>85.59999999999999</v>
+      </c>
+      <c r="G1524" t="n">
+        <v>74.8</v>
+      </c>
+      <c r="H1524" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="1525" spans="1:8">
       <c r="A1525" s="1" t="n">
@@ -45529,12 +45805,24 @@
       <c r="B1525" t="s">
         <v>890</v>
       </c>
-      <c r="C1525" t="s"/>
-      <c r="D1525" t="s"/>
-      <c r="E1525" t="s"/>
-      <c r="F1525" t="s"/>
-      <c r="G1525" t="s"/>
-      <c r="H1525" t="s"/>
+      <c r="C1525" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="D1525" t="n">
+        <v>59.5</v>
+      </c>
+      <c r="E1525" t="n">
+        <v>31</v>
+      </c>
+      <c r="F1525" t="n">
+        <v>30.9</v>
+      </c>
+      <c r="G1525" t="n">
+        <v>36.7</v>
+      </c>
+      <c r="H1525" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="1526" spans="1:8">
       <c r="A1526" s="1" t="n">
@@ -45543,12 +45831,24 @@
       <c r="B1526" t="s">
         <v>201</v>
       </c>
-      <c r="C1526" t="s"/>
-      <c r="D1526" t="s"/>
-      <c r="E1526" t="s"/>
-      <c r="F1526" t="s"/>
-      <c r="G1526" t="s"/>
-      <c r="H1526" t="s"/>
+      <c r="C1526" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="D1526" t="n">
+        <v>88.40000000000001</v>
+      </c>
+      <c r="E1526" t="n">
+        <v>107.3</v>
+      </c>
+      <c r="F1526" t="n">
+        <v>115.8</v>
+      </c>
+      <c r="G1526" t="n">
+        <v>97.3</v>
+      </c>
+      <c r="H1526" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="1527" spans="1:8">
       <c r="A1527" s="1" t="n">
@@ -45557,12 +45857,24 @@
       <c r="B1527" t="s">
         <v>247</v>
       </c>
-      <c r="C1527" t="s"/>
-      <c r="D1527" t="s"/>
-      <c r="E1527" t="s"/>
-      <c r="F1527" t="s"/>
-      <c r="G1527" t="s"/>
-      <c r="H1527" t="s"/>
+      <c r="C1527" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="D1527" t="n">
+        <v>101</v>
+      </c>
+      <c r="E1527" t="n">
+        <v>67.59999999999999</v>
+      </c>
+      <c r="F1527" t="n">
+        <v>60.3</v>
+      </c>
+      <c r="G1527" t="n">
+        <v>71.59999999999999</v>
+      </c>
+      <c r="H1527" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="1528" spans="1:8">
       <c r="A1528" s="1" t="n">
@@ -45571,12 +45883,24 @@
       <c r="B1528" t="s">
         <v>194</v>
       </c>
-      <c r="C1528" t="s"/>
-      <c r="D1528" t="s"/>
-      <c r="E1528" t="s"/>
-      <c r="F1528" t="s"/>
-      <c r="G1528" t="s"/>
-      <c r="H1528" t="s"/>
+      <c r="C1528" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="D1528" t="n">
+        <v>100.3</v>
+      </c>
+      <c r="E1528" t="n">
+        <v>67.59999999999999</v>
+      </c>
+      <c r="F1528" t="n">
+        <v>83.09999999999999</v>
+      </c>
+      <c r="G1528" t="n">
+        <v>75</v>
+      </c>
+      <c r="H1528" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="1529" spans="1:8">
       <c r="A1529" s="1" t="n">
@@ -46729,12 +47053,24 @@
       <c r="B1573" t="s">
         <v>195</v>
       </c>
-      <c r="C1573" t="s"/>
-      <c r="D1573" t="s"/>
-      <c r="E1573" t="s"/>
-      <c r="F1573" t="s"/>
-      <c r="G1573" t="s"/>
-      <c r="H1573" t="s"/>
+      <c r="C1573" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="D1573" t="n">
+        <v>87.3</v>
+      </c>
+      <c r="E1573" t="n">
+        <v>106.4</v>
+      </c>
+      <c r="F1573" t="n">
+        <v>90.7</v>
+      </c>
+      <c r="G1573" t="n">
+        <v>81.7</v>
+      </c>
+      <c r="H1573" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="1574" spans="1:8">
       <c r="A1574" s="1" t="n">
@@ -46743,12 +47079,24 @@
       <c r="B1574" t="s">
         <v>200</v>
       </c>
-      <c r="C1574" t="s"/>
-      <c r="D1574" t="s"/>
-      <c r="E1574" t="s"/>
-      <c r="F1574" t="s"/>
-      <c r="G1574" t="s"/>
-      <c r="H1574" t="s"/>
+      <c r="C1574" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="D1574" t="n">
+        <v>87.3</v>
+      </c>
+      <c r="E1574" t="n">
+        <v>106.7</v>
+      </c>
+      <c r="F1574" t="n">
+        <v>103.7</v>
+      </c>
+      <c r="G1574" t="n">
+        <v>95.09999999999999</v>
+      </c>
+      <c r="H1574" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="1575" spans="1:8">
       <c r="A1575" s="1" t="n">
@@ -46757,12 +47105,24 @@
       <c r="B1575" t="s">
         <v>195</v>
       </c>
-      <c r="C1575" t="s"/>
-      <c r="D1575" t="s"/>
-      <c r="E1575" t="s"/>
-      <c r="F1575" t="s"/>
-      <c r="G1575" t="s"/>
-      <c r="H1575" t="s"/>
+      <c r="C1575" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="D1575" t="n">
+        <v>87.90000000000001</v>
+      </c>
+      <c r="E1575" t="n">
+        <v>79.8</v>
+      </c>
+      <c r="F1575" t="n">
+        <v>97.2</v>
+      </c>
+      <c r="G1575" t="n">
+        <v>59</v>
+      </c>
+      <c r="H1575" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="1576" spans="1:8">
       <c r="A1576" s="1" t="n">
@@ -46771,12 +47131,24 @@
       <c r="B1576" t="s">
         <v>195</v>
       </c>
-      <c r="C1576" t="s"/>
-      <c r="D1576" t="s"/>
-      <c r="E1576" t="s"/>
-      <c r="F1576" t="s"/>
-      <c r="G1576" t="s"/>
-      <c r="H1576" t="s"/>
+      <c r="C1576" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="D1576" t="n">
+        <v>99</v>
+      </c>
+      <c r="E1576" t="n">
+        <v>79.5</v>
+      </c>
+      <c r="F1576" t="n">
+        <v>74.5</v>
+      </c>
+      <c r="G1576" t="n">
+        <v>82.8</v>
+      </c>
+      <c r="H1576" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="1577" spans="1:8">
       <c r="A1577" s="1" t="n">
@@ -48761,12 +49133,24 @@
       <c r="B1653" t="s">
         <v>195</v>
       </c>
-      <c r="C1653" t="s"/>
-      <c r="D1653" t="s"/>
-      <c r="E1653" t="s"/>
-      <c r="F1653" t="s"/>
-      <c r="G1653" t="s"/>
-      <c r="H1653" t="s"/>
+      <c r="C1653" t="n">
+        <v>5</v>
+      </c>
+      <c r="D1653" t="n">
+        <v>99.5</v>
+      </c>
+      <c r="E1653" t="n">
+        <v>114.9</v>
+      </c>
+      <c r="F1653" t="n">
+        <v>93.2</v>
+      </c>
+      <c r="G1653" t="n">
+        <v>91.5</v>
+      </c>
+      <c r="H1653" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="1654" spans="1:8">
       <c r="A1654" s="1" t="n">
@@ -48775,12 +49159,24 @@
       <c r="B1654" t="s">
         <v>247</v>
       </c>
-      <c r="C1654" t="s"/>
-      <c r="D1654" t="s"/>
-      <c r="E1654" t="s"/>
-      <c r="F1654" t="s"/>
-      <c r="G1654" t="s"/>
-      <c r="H1654" t="s"/>
+      <c r="C1654" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="D1654" t="n">
+        <v>113.2</v>
+      </c>
+      <c r="E1654" t="n">
+        <v>88.7</v>
+      </c>
+      <c r="F1654" t="n">
+        <v>82.2</v>
+      </c>
+      <c r="G1654" t="n">
+        <v>82.5</v>
+      </c>
+      <c r="H1654" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="1655" spans="1:8">
       <c r="A1655" s="1" t="n">
@@ -48789,12 +49185,24 @@
       <c r="B1655" t="s">
         <v>194</v>
       </c>
-      <c r="C1655" t="s"/>
-      <c r="D1655" t="s"/>
-      <c r="E1655" t="s"/>
-      <c r="F1655" t="s"/>
-      <c r="G1655" t="s"/>
-      <c r="H1655" t="s"/>
+      <c r="C1655" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="D1655" t="n">
+        <v>100.6</v>
+      </c>
+      <c r="E1655" t="n">
+        <v>90.8</v>
+      </c>
+      <c r="F1655" t="n">
+        <v>70.09999999999999</v>
+      </c>
+      <c r="G1655" t="n">
+        <v>138.6</v>
+      </c>
+      <c r="H1655" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="1656" spans="1:8">
       <c r="A1656" s="1" t="n">
@@ -48803,12 +49211,24 @@
       <c r="B1656" t="s">
         <v>194</v>
       </c>
-      <c r="C1656" t="s"/>
-      <c r="D1656" t="s"/>
-      <c r="E1656" t="s"/>
-      <c r="F1656" t="s"/>
-      <c r="G1656" t="s"/>
-      <c r="H1656" t="s"/>
+      <c r="C1656" t="n">
+        <v>5</v>
+      </c>
+      <c r="D1656" t="n">
+        <v>100.6</v>
+      </c>
+      <c r="E1656" t="n">
+        <v>105.6</v>
+      </c>
+      <c r="F1656" t="n">
+        <v>103.7</v>
+      </c>
+      <c r="G1656" t="n">
+        <v>92.8</v>
+      </c>
+      <c r="H1656" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="1657" spans="1:8">
       <c r="A1657" s="1" t="n">
@@ -48817,12 +49237,24 @@
       <c r="B1657" t="s">
         <v>200</v>
       </c>
-      <c r="C1657" t="s"/>
-      <c r="D1657" t="s"/>
-      <c r="E1657" t="s"/>
-      <c r="F1657" t="s"/>
-      <c r="G1657" t="s"/>
-      <c r="H1657" t="s"/>
+      <c r="C1657" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="D1657" t="n">
+        <v>100.6</v>
+      </c>
+      <c r="E1657" t="n">
+        <v>85.2</v>
+      </c>
+      <c r="F1657" t="n">
+        <v>76.7</v>
+      </c>
+      <c r="G1657" t="n">
+        <v>88.7</v>
+      </c>
+      <c r="H1657" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="1658" spans="1:8">
       <c r="A1658" s="1" t="n">
@@ -48831,12 +49263,24 @@
       <c r="B1658" t="s">
         <v>194</v>
       </c>
-      <c r="C1658" t="s"/>
-      <c r="D1658" t="s"/>
-      <c r="E1658" t="s"/>
-      <c r="F1658" t="s"/>
-      <c r="G1658" t="s"/>
-      <c r="H1658" t="s"/>
+      <c r="C1658" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="D1658" t="n">
+        <v>101.8</v>
+      </c>
+      <c r="E1658" t="n">
+        <v>91.90000000000001</v>
+      </c>
+      <c r="F1658" t="n">
+        <v>68.40000000000001</v>
+      </c>
+      <c r="G1658" t="n">
+        <v>77.40000000000001</v>
+      </c>
+      <c r="H1658" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="1659" spans="1:8">
       <c r="A1659" s="1" t="n">
@@ -50483,12 +50927,24 @@
       <c r="B1722" t="s">
         <v>201</v>
       </c>
-      <c r="C1722" t="s"/>
-      <c r="D1722" t="s"/>
-      <c r="E1722" t="s"/>
-      <c r="F1722" t="s"/>
-      <c r="G1722" t="s"/>
-      <c r="H1722" t="s"/>
+      <c r="C1722" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="D1722" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1722" t="n">
+        <v>64.59999999999999</v>
+      </c>
+      <c r="F1722" t="n">
+        <v>72.90000000000001</v>
+      </c>
+      <c r="G1722" t="n">
+        <v>67.2</v>
+      </c>
+      <c r="H1722" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="1723" spans="1:8">
       <c r="A1723" s="1" t="n">
@@ -50497,12 +50953,24 @@
       <c r="B1723" t="s">
         <v>247</v>
       </c>
-      <c r="C1723" t="s"/>
-      <c r="D1723" t="s"/>
-      <c r="E1723" t="s"/>
-      <c r="F1723" t="s"/>
-      <c r="G1723" t="s"/>
-      <c r="H1723" t="s"/>
+      <c r="C1723" t="n">
+        <v>5</v>
+      </c>
+      <c r="D1723" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1723" t="n">
+        <v>103.1</v>
+      </c>
+      <c r="F1723" t="n">
+        <v>106.8</v>
+      </c>
+      <c r="G1723" t="n">
+        <v>92.09999999999999</v>
+      </c>
+      <c r="H1723" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="1724" spans="1:8">
       <c r="A1724" s="1" t="n">
@@ -50511,12 +50979,24 @@
       <c r="B1724" t="s">
         <v>197</v>
       </c>
-      <c r="C1724" t="s"/>
-      <c r="D1724" t="s"/>
-      <c r="E1724" t="s"/>
-      <c r="F1724" t="s"/>
-      <c r="G1724" t="s"/>
-      <c r="H1724" t="s"/>
+      <c r="C1724" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="D1724" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1724" t="n">
+        <v>59.5</v>
+      </c>
+      <c r="F1724" t="n">
+        <v>69.8</v>
+      </c>
+      <c r="G1724" t="n">
+        <v>63.9</v>
+      </c>
+      <c r="H1724" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="1725" spans="1:8">
       <c r="A1725" s="1" t="n">
@@ -57191,12 +57671,24 @@
       <c r="B1982" t="s">
         <v>200</v>
       </c>
-      <c r="C1982" t="s"/>
-      <c r="D1982" t="s"/>
-      <c r="E1982" t="s"/>
-      <c r="F1982" t="s"/>
-      <c r="G1982" t="s"/>
-      <c r="H1982" t="s"/>
+      <c r="C1982" t="n">
+        <v>3</v>
+      </c>
+      <c r="D1982" t="n">
+        <v>64.7</v>
+      </c>
+      <c r="E1982" t="n">
+        <v>65.8</v>
+      </c>
+      <c r="F1982" t="n">
+        <v>58.8</v>
+      </c>
+      <c r="G1982" t="n">
+        <v>52</v>
+      </c>
+      <c r="H1982" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="1983" spans="1:8">
       <c r="A1983" s="1" t="n">
@@ -57205,12 +57697,24 @@
       <c r="B1983" t="s">
         <v>195</v>
       </c>
-      <c r="C1983" t="s"/>
-      <c r="D1983" t="s"/>
-      <c r="E1983" t="s"/>
-      <c r="F1983" t="s"/>
-      <c r="G1983" t="s"/>
-      <c r="H1983" t="s"/>
+      <c r="C1983" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="D1983" t="n">
+        <v>79.59999999999999</v>
+      </c>
+      <c r="E1983" t="n">
+        <v>66.5</v>
+      </c>
+      <c r="F1983" t="n">
+        <v>63.4</v>
+      </c>
+      <c r="G1983" t="n">
+        <v>57.4</v>
+      </c>
+      <c r="H1983" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="1984" spans="1:8">
       <c r="A1984" s="1" t="n">
@@ -57219,12 +57723,24 @@
       <c r="B1984" t="s">
         <v>890</v>
       </c>
-      <c r="C1984" t="s"/>
-      <c r="D1984" t="s"/>
-      <c r="E1984" t="s"/>
-      <c r="F1984" t="s"/>
-      <c r="G1984" t="s"/>
-      <c r="H1984" t="s"/>
+      <c r="C1984" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="D1984" t="n">
+        <v>59.2</v>
+      </c>
+      <c r="E1984" t="n">
+        <v>38.6</v>
+      </c>
+      <c r="F1984" t="n">
+        <v>31.4</v>
+      </c>
+      <c r="G1984" t="n">
+        <v>32.4</v>
+      </c>
+      <c r="H1984" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="1985" spans="1:8">
       <c r="A1985" s="1" t="n">
@@ -57233,12 +57749,24 @@
       <c r="B1985" t="s">
         <v>195</v>
       </c>
-      <c r="C1985" t="s"/>
-      <c r="D1985" t="s"/>
-      <c r="E1985" t="s"/>
-      <c r="F1985" t="s"/>
-      <c r="G1985" t="s"/>
-      <c r="H1985" t="s"/>
+      <c r="C1985" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="D1985" t="n">
+        <v>89.5</v>
+      </c>
+      <c r="E1985" t="n">
+        <v>105.4</v>
+      </c>
+      <c r="F1985" t="n">
+        <v>107.4</v>
+      </c>
+      <c r="G1985" t="n">
+        <v>102.7</v>
+      </c>
+      <c r="H1985" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="1986" spans="1:8">
       <c r="A1986" s="1" t="n">
@@ -57247,12 +57775,24 @@
       <c r="B1986" t="s">
         <v>247</v>
       </c>
-      <c r="C1986" t="s"/>
-      <c r="D1986" t="s"/>
-      <c r="E1986" t="s"/>
-      <c r="F1986" t="s"/>
-      <c r="G1986" t="s"/>
-      <c r="H1986" t="s"/>
+      <c r="C1986" t="n">
+        <v>4</v>
+      </c>
+      <c r="D1986" t="n">
+        <v>92.5</v>
+      </c>
+      <c r="E1986" t="n">
+        <v>71.5</v>
+      </c>
+      <c r="F1986" t="n">
+        <v>86.2</v>
+      </c>
+      <c r="G1986" t="n">
+        <v>64.2</v>
+      </c>
+      <c r="H1986" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="1987" spans="1:8">
       <c r="A1987" s="1" t="n">
@@ -58223,12 +58763,24 @@
       <c r="B2024" t="s">
         <v>1057</v>
       </c>
-      <c r="C2024" t="s"/>
-      <c r="D2024" t="s"/>
-      <c r="E2024" t="s"/>
-      <c r="F2024" t="s"/>
-      <c r="G2024" t="s"/>
-      <c r="H2024" t="s"/>
+      <c r="C2024" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="D2024" t="n">
+        <v>112.5</v>
+      </c>
+      <c r="E2024" t="n">
+        <v>70.5</v>
+      </c>
+      <c r="F2024" t="n">
+        <v>83</v>
+      </c>
+      <c r="G2024" t="n">
+        <v>60.7</v>
+      </c>
+      <c r="H2024" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2025" spans="1:8">
       <c r="A2025" s="1" t="n">
@@ -58237,12 +58789,24 @@
       <c r="B2025" t="s">
         <v>1057</v>
       </c>
-      <c r="C2025" t="s"/>
-      <c r="D2025" t="s"/>
-      <c r="E2025" t="s"/>
-      <c r="F2025" t="s"/>
-      <c r="G2025" t="s"/>
-      <c r="H2025" t="s"/>
+      <c r="C2025" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="D2025" t="n">
+        <v>122.3</v>
+      </c>
+      <c r="E2025" t="n">
+        <v>81.3</v>
+      </c>
+      <c r="F2025" t="n">
+        <v>79.90000000000001</v>
+      </c>
+      <c r="G2025" t="n">
+        <v>86.8</v>
+      </c>
+      <c r="H2025" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2026" spans="1:8">
       <c r="A2026" s="1" t="n">
@@ -58251,12 +58815,24 @@
       <c r="B2026" t="s">
         <v>194</v>
       </c>
-      <c r="C2026" t="s"/>
-      <c r="D2026" t="s"/>
-      <c r="E2026" t="s"/>
-      <c r="F2026" t="s"/>
-      <c r="G2026" t="s"/>
-      <c r="H2026" t="s"/>
+      <c r="C2026" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="D2026" t="n">
+        <v>53</v>
+      </c>
+      <c r="E2026" t="n">
+        <v>60</v>
+      </c>
+      <c r="F2026" t="n">
+        <v>47.4</v>
+      </c>
+      <c r="G2026" t="n">
+        <v>63.7</v>
+      </c>
+      <c r="H2026" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2027" spans="1:8">
       <c r="A2027" s="1" t="n">
@@ -58265,12 +58841,24 @@
       <c r="B2027" t="s">
         <v>890</v>
       </c>
-      <c r="C2027" t="s"/>
-      <c r="D2027" t="s"/>
-      <c r="E2027" t="s"/>
-      <c r="F2027" t="s"/>
-      <c r="G2027" t="s"/>
-      <c r="H2027" t="s"/>
+      <c r="C2027" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="D2027" t="n">
+        <v>59.2</v>
+      </c>
+      <c r="E2027" t="n">
+        <v>45.9</v>
+      </c>
+      <c r="F2027" t="n">
+        <v>46.2</v>
+      </c>
+      <c r="G2027" t="n">
+        <v>62.3</v>
+      </c>
+      <c r="H2027" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2028" spans="1:8">
       <c r="A2028" s="1" t="n">
@@ -58279,12 +58867,24 @@
       <c r="B2028" t="s">
         <v>1057</v>
       </c>
-      <c r="C2028" t="s"/>
-      <c r="D2028" t="s"/>
-      <c r="E2028" t="s"/>
-      <c r="F2028" t="s"/>
-      <c r="G2028" t="s"/>
-      <c r="H2028" t="s"/>
+      <c r="C2028" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="D2028" t="n">
+        <v>122.3</v>
+      </c>
+      <c r="E2028" t="n">
+        <v>83.5</v>
+      </c>
+      <c r="F2028" t="n">
+        <v>111.5</v>
+      </c>
+      <c r="G2028" t="n">
+        <v>89</v>
+      </c>
+      <c r="H2028" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2029" spans="1:8">
       <c r="A2029" s="1" t="n">
@@ -58865,12 +59465,24 @@
       <c r="B2051" t="s">
         <v>195</v>
       </c>
-      <c r="C2051" t="s"/>
-      <c r="D2051" t="s"/>
-      <c r="E2051" t="s"/>
-      <c r="F2051" t="s"/>
-      <c r="G2051" t="s"/>
-      <c r="H2051" t="s"/>
+      <c r="C2051" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="D2051" t="n">
+        <v>95.7</v>
+      </c>
+      <c r="E2051" t="n">
+        <v>26.4</v>
+      </c>
+      <c r="F2051" t="n">
+        <v>18.9</v>
+      </c>
+      <c r="G2051" t="n">
+        <v>39.9</v>
+      </c>
+      <c r="H2051" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2052" spans="1:8">
       <c r="A2052" s="1" t="n">
@@ -58879,12 +59491,24 @@
       <c r="B2052" t="s">
         <v>195</v>
       </c>
-      <c r="C2052" t="s"/>
-      <c r="D2052" t="s"/>
-      <c r="E2052" t="s"/>
-      <c r="F2052" t="s"/>
-      <c r="G2052" t="s"/>
-      <c r="H2052" t="s"/>
+      <c r="C2052" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="D2052" t="n">
+        <v>58.2</v>
+      </c>
+      <c r="E2052" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="F2052" t="n">
+        <v>16.7</v>
+      </c>
+      <c r="G2052" t="n">
+        <v>20.1</v>
+      </c>
+      <c r="H2052" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2053" spans="1:8">
       <c r="A2053" s="1" t="n">
@@ -58893,12 +59517,24 @@
       <c r="B2053" t="s">
         <v>195</v>
       </c>
-      <c r="C2053" t="s"/>
-      <c r="D2053" t="s"/>
-      <c r="E2053" t="s"/>
-      <c r="F2053" t="s"/>
-      <c r="G2053" t="s"/>
-      <c r="H2053" t="s"/>
+      <c r="C2053" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="D2053" t="n">
+        <v>101</v>
+      </c>
+      <c r="E2053" t="n">
+        <v>19</v>
+      </c>
+      <c r="F2053" t="n">
+        <v>12.6</v>
+      </c>
+      <c r="G2053" t="n">
+        <v>46.9</v>
+      </c>
+      <c r="H2053" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2054" spans="1:8">
       <c r="A2054" s="1" t="n">
@@ -58907,12 +59543,24 @@
       <c r="B2054" t="s">
         <v>195</v>
       </c>
-      <c r="C2054" t="s"/>
-      <c r="D2054" t="s"/>
-      <c r="E2054" t="s"/>
-      <c r="F2054" t="s"/>
-      <c r="G2054" t="s"/>
-      <c r="H2054" t="s"/>
+      <c r="C2054" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="D2054" t="n">
+        <v>100.6</v>
+      </c>
+      <c r="E2054" t="n">
+        <v>76.5</v>
+      </c>
+      <c r="F2054" t="n">
+        <v>103</v>
+      </c>
+      <c r="G2054" t="n">
+        <v>67.3</v>
+      </c>
+      <c r="H2054" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2055" spans="1:8">
       <c r="A2055" s="1" t="n">
@@ -58921,12 +59569,24 @@
       <c r="B2055" t="s">
         <v>195</v>
       </c>
-      <c r="C2055" t="s"/>
-      <c r="D2055" t="s"/>
-      <c r="E2055" t="s"/>
-      <c r="F2055" t="s"/>
-      <c r="G2055" t="s"/>
-      <c r="H2055" t="s"/>
+      <c r="C2055" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="D2055" t="n">
+        <v>101</v>
+      </c>
+      <c r="E2055" t="n">
+        <v>66.90000000000001</v>
+      </c>
+      <c r="F2055" t="n">
+        <v>96.40000000000001</v>
+      </c>
+      <c r="G2055" t="n">
+        <v>63.8</v>
+      </c>
+      <c r="H2055" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2056" spans="1:8">
       <c r="A2056" s="1" t="n">
@@ -61353,12 +62013,24 @@
       <c r="B2149" t="s">
         <v>195</v>
       </c>
-      <c r="C2149" t="s"/>
-      <c r="D2149" t="s"/>
-      <c r="E2149" t="s"/>
-      <c r="F2149" t="s"/>
-      <c r="G2149" t="s"/>
-      <c r="H2149" t="s"/>
+      <c r="C2149" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="D2149" t="n">
+        <v>107.1</v>
+      </c>
+      <c r="E2149" t="n">
+        <v>96</v>
+      </c>
+      <c r="F2149" t="n">
+        <v>93.2</v>
+      </c>
+      <c r="G2149" t="n">
+        <v>80.7</v>
+      </c>
+      <c r="H2149" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2150" spans="1:8">
       <c r="A2150" s="1" t="n">
@@ -61367,12 +62039,24 @@
       <c r="B2150" t="s">
         <v>247</v>
       </c>
-      <c r="C2150" t="s"/>
-      <c r="D2150" t="s"/>
-      <c r="E2150" t="s"/>
-      <c r="F2150" t="s"/>
-      <c r="G2150" t="s"/>
-      <c r="H2150" t="s"/>
+      <c r="C2150" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="D2150" t="n">
+        <v>80.5</v>
+      </c>
+      <c r="E2150" t="n">
+        <v>66.3</v>
+      </c>
+      <c r="F2150" t="n">
+        <v>59.7</v>
+      </c>
+      <c r="G2150" t="n">
+        <v>57.1</v>
+      </c>
+      <c r="H2150" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2151" spans="1:8">
       <c r="A2151" s="1" t="n">
@@ -61381,12 +62065,24 @@
       <c r="B2151" t="s">
         <v>201</v>
       </c>
-      <c r="C2151" t="s"/>
-      <c r="D2151" t="s"/>
-      <c r="E2151" t="s"/>
-      <c r="F2151" t="s"/>
-      <c r="G2151" t="s"/>
-      <c r="H2151" t="s"/>
+      <c r="C2151" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="D2151" t="n">
+        <v>51.7</v>
+      </c>
+      <c r="E2151" t="n">
+        <v>34.9</v>
+      </c>
+      <c r="F2151" t="n">
+        <v>36.3</v>
+      </c>
+      <c r="G2151" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2151" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2152" spans="1:8">
       <c r="A2152" s="1" t="n">
@@ -61395,12 +62091,24 @@
       <c r="B2152" t="s">
         <v>195</v>
       </c>
-      <c r="C2152" t="s"/>
-      <c r="D2152" t="s"/>
-      <c r="E2152" t="s"/>
-      <c r="F2152" t="s"/>
-      <c r="G2152" t="s"/>
-      <c r="H2152" t="s"/>
+      <c r="C2152" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="D2152" t="n">
+        <v>92.5</v>
+      </c>
+      <c r="E2152" t="n">
+        <v>77.59999999999999</v>
+      </c>
+      <c r="F2152" t="n">
+        <v>70.09999999999999</v>
+      </c>
+      <c r="G2152" t="n">
+        <v>72.7</v>
+      </c>
+      <c r="H2152" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2153" spans="1:8">
       <c r="A2153" s="1" t="n">
@@ -61409,12 +62117,24 @@
       <c r="B2153" t="s">
         <v>247</v>
       </c>
-      <c r="C2153" t="s"/>
-      <c r="D2153" t="s"/>
-      <c r="E2153" t="s"/>
-      <c r="F2153" t="s"/>
-      <c r="G2153" t="s"/>
-      <c r="H2153" t="s"/>
+      <c r="C2153" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="D2153" t="n">
+        <v>80</v>
+      </c>
+      <c r="E2153" t="n">
+        <v>78.90000000000001</v>
+      </c>
+      <c r="F2153" t="n">
+        <v>100.5</v>
+      </c>
+      <c r="G2153" t="n">
+        <v>71.2</v>
+      </c>
+      <c r="H2153" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2154" spans="1:8">
       <c r="A2154" s="1" t="n">
@@ -68703,12 +69423,24 @@
       <c r="B2434" t="s">
         <v>1291</v>
       </c>
-      <c r="C2434" t="s"/>
-      <c r="D2434" t="s"/>
-      <c r="E2434" t="s"/>
-      <c r="F2434" t="s"/>
-      <c r="G2434" t="s"/>
-      <c r="H2434" t="s"/>
+      <c r="C2434" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="D2434" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2434" t="n">
+        <v>44.8</v>
+      </c>
+      <c r="F2434" t="n">
+        <v>41.9</v>
+      </c>
+      <c r="G2434" t="n">
+        <v>50.6</v>
+      </c>
+      <c r="H2434" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2435" spans="1:8">
       <c r="A2435" s="1" t="n">
@@ -68717,12 +69449,24 @@
       <c r="B2435" t="s">
         <v>890</v>
       </c>
-      <c r="C2435" t="s"/>
-      <c r="D2435" t="s"/>
-      <c r="E2435" t="s"/>
-      <c r="F2435" t="s"/>
-      <c r="G2435" t="s"/>
-      <c r="H2435" t="s"/>
+      <c r="C2435" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="D2435" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2435" t="n">
+        <v>67.40000000000001</v>
+      </c>
+      <c r="F2435" t="n">
+        <v>62.8</v>
+      </c>
+      <c r="G2435" t="n">
+        <v>62.7</v>
+      </c>
+      <c r="H2435" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2436" spans="1:8">
       <c r="A2436" s="1" t="n">
@@ -68731,12 +69475,24 @@
       <c r="B2436" t="s">
         <v>890</v>
       </c>
-      <c r="C2436" t="s"/>
-      <c r="D2436" t="s"/>
-      <c r="E2436" t="s"/>
-      <c r="F2436" t="s"/>
-      <c r="G2436" t="s"/>
-      <c r="H2436" t="s"/>
+      <c r="C2436" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="D2436" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2436" t="n">
+        <v>56.7</v>
+      </c>
+      <c r="F2436" t="n">
+        <v>36.8</v>
+      </c>
+      <c r="G2436" t="n">
+        <v>65.59999999999999</v>
+      </c>
+      <c r="H2436" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2437" spans="1:8">
       <c r="A2437" s="1" t="n">
@@ -68745,12 +69501,24 @@
       <c r="B2437" t="s">
         <v>890</v>
       </c>
-      <c r="C2437" t="s"/>
-      <c r="D2437" t="s"/>
-      <c r="E2437" t="s"/>
-      <c r="F2437" t="s"/>
-      <c r="G2437" t="s"/>
-      <c r="H2437" t="s"/>
+      <c r="C2437" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="D2437" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2437" t="n">
+        <v>58.2</v>
+      </c>
+      <c r="F2437" t="n">
+        <v>47.9</v>
+      </c>
+      <c r="G2437" t="n">
+        <v>59.5</v>
+      </c>
+      <c r="H2437" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2438" spans="1:8">
       <c r="A2438" s="1" t="n">
@@ -68759,12 +69527,24 @@
       <c r="B2438" t="s">
         <v>1292</v>
       </c>
-      <c r="C2438" t="s"/>
-      <c r="D2438" t="s"/>
-      <c r="E2438" t="s"/>
-      <c r="F2438" t="s"/>
-      <c r="G2438" t="s"/>
-      <c r="H2438" t="s"/>
+      <c r="C2438" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="D2438" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2438" t="n">
+        <v>59.4</v>
+      </c>
+      <c r="F2438" t="n">
+        <v>39.1</v>
+      </c>
+      <c r="G2438" t="n">
+        <v>54.6</v>
+      </c>
+      <c r="H2438" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2439" spans="1:8">
       <c r="A2439" s="1" t="n">
@@ -68773,12 +69553,24 @@
       <c r="B2439" t="s">
         <v>1292</v>
       </c>
-      <c r="C2439" t="s"/>
-      <c r="D2439" t="s"/>
-      <c r="E2439" t="s"/>
-      <c r="F2439" t="s"/>
-      <c r="G2439" t="s"/>
-      <c r="H2439" t="s"/>
+      <c r="C2439" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="D2439" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2439" t="n">
+        <v>68.59999999999999</v>
+      </c>
+      <c r="F2439" t="n">
+        <v>69.09999999999999</v>
+      </c>
+      <c r="G2439" t="n">
+        <v>50.6</v>
+      </c>
+      <c r="H2439" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2440" spans="1:8">
       <c r="A2440" s="1" t="n">
@@ -68787,12 +69579,24 @@
       <c r="B2440" t="s">
         <v>1292</v>
       </c>
-      <c r="C2440" t="s"/>
-      <c r="D2440" t="s"/>
-      <c r="E2440" t="s"/>
-      <c r="F2440" t="s"/>
-      <c r="G2440" t="s"/>
-      <c r="H2440" t="s"/>
+      <c r="C2440" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="D2440" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2440" t="n">
+        <v>22.1</v>
+      </c>
+      <c r="F2440" t="n">
+        <v>20.3</v>
+      </c>
+      <c r="G2440" t="n">
+        <v>34.9</v>
+      </c>
+      <c r="H2440" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2441" spans="1:8">
       <c r="A2441" s="1" t="n">
@@ -68801,12 +69605,24 @@
       <c r="B2441" t="s">
         <v>1292</v>
       </c>
-      <c r="C2441" t="s"/>
-      <c r="D2441" t="s"/>
-      <c r="E2441" t="s"/>
-      <c r="F2441" t="s"/>
-      <c r="G2441" t="s"/>
-      <c r="H2441" t="s"/>
+      <c r="C2441" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="D2441" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2441" t="n">
+        <v>74.5</v>
+      </c>
+      <c r="F2441" t="n">
+        <v>58.7</v>
+      </c>
+      <c r="G2441" t="n">
+        <v>69.5</v>
+      </c>
+      <c r="H2441" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2442" spans="1:8">
       <c r="A2442" s="1" t="n">
@@ -68815,12 +69631,24 @@
       <c r="B2442" t="s">
         <v>1292</v>
       </c>
-      <c r="C2442" t="s"/>
-      <c r="D2442" t="s"/>
-      <c r="E2442" t="s"/>
-      <c r="F2442" t="s"/>
-      <c r="G2442" t="s"/>
-      <c r="H2442" t="s"/>
+      <c r="C2442" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="D2442" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2442" t="n">
+        <v>45.1</v>
+      </c>
+      <c r="F2442" t="n">
+        <v>50</v>
+      </c>
+      <c r="G2442" t="n">
+        <v>43</v>
+      </c>
+      <c r="H2442" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2443" spans="1:8">
       <c r="A2443" s="1" t="n">
@@ -68829,12 +69657,24 @@
       <c r="B2443" t="s">
         <v>890</v>
       </c>
-      <c r="C2443" t="s"/>
-      <c r="D2443" t="s"/>
-      <c r="E2443" t="s"/>
-      <c r="F2443" t="s"/>
-      <c r="G2443" t="s"/>
-      <c r="H2443" t="s"/>
+      <c r="C2443" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="D2443" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2443" t="n">
+        <v>57.5</v>
+      </c>
+      <c r="F2443" t="n">
+        <v>41.2</v>
+      </c>
+      <c r="G2443" t="n">
+        <v>40.9</v>
+      </c>
+      <c r="H2443" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2444" spans="1:8">
       <c r="A2444" s="1" t="n">
@@ -68843,12 +69683,24 @@
       <c r="B2444" t="s">
         <v>1292</v>
       </c>
-      <c r="C2444" t="s"/>
-      <c r="D2444" t="s"/>
-      <c r="E2444" t="s"/>
-      <c r="F2444" t="s"/>
-      <c r="G2444" t="s"/>
-      <c r="H2444" t="s"/>
+      <c r="C2444" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="D2444" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2444" t="n">
+        <v>64.59999999999999</v>
+      </c>
+      <c r="F2444" t="n">
+        <v>47</v>
+      </c>
+      <c r="G2444" t="n">
+        <v>51.9</v>
+      </c>
+      <c r="H2444" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2445" spans="1:8">
       <c r="A2445" s="1" t="n">
@@ -68857,12 +69709,24 @@
       <c r="B2445" t="s">
         <v>197</v>
       </c>
-      <c r="C2445" t="s"/>
-      <c r="D2445" t="s"/>
-      <c r="E2445" t="s"/>
-      <c r="F2445" t="s"/>
-      <c r="G2445" t="s"/>
-      <c r="H2445" t="s"/>
+      <c r="C2445" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="D2445" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2445" t="n">
+        <v>37.8</v>
+      </c>
+      <c r="F2445" t="n">
+        <v>30.8</v>
+      </c>
+      <c r="G2445" t="n">
+        <v>42.4</v>
+      </c>
+      <c r="H2445" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2446" spans="1:8">
       <c r="A2446" s="1" t="n">
@@ -68871,12 +69735,24 @@
       <c r="B2446" t="s">
         <v>1291</v>
       </c>
-      <c r="C2446" t="s"/>
-      <c r="D2446" t="s"/>
-      <c r="E2446" t="s"/>
-      <c r="F2446" t="s"/>
-      <c r="G2446" t="s"/>
-      <c r="H2446" t="s"/>
+      <c r="C2446" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="D2446" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2446" t="n">
+        <v>23.9</v>
+      </c>
+      <c r="F2446" t="n">
+        <v>26.7</v>
+      </c>
+      <c r="G2446" t="n">
+        <v>33.8</v>
+      </c>
+      <c r="H2446" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2447" spans="1:8">
       <c r="A2447" s="1" t="n">
@@ -68885,12 +69761,24 @@
       <c r="B2447" t="s">
         <v>1292</v>
       </c>
-      <c r="C2447" t="s"/>
-      <c r="D2447" t="s"/>
-      <c r="E2447" t="s"/>
-      <c r="F2447" t="s"/>
-      <c r="G2447" t="s"/>
-      <c r="H2447" t="s"/>
+      <c r="C2447" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="D2447" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2447" t="n">
+        <v>62.1</v>
+      </c>
+      <c r="F2447" t="n">
+        <v>40.7</v>
+      </c>
+      <c r="G2447" t="n">
+        <v>59.9</v>
+      </c>
+      <c r="H2447" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2448" spans="1:8">
       <c r="A2448" s="1" t="n">
@@ -68899,12 +69787,24 @@
       <c r="B2448" t="s">
         <v>1291</v>
       </c>
-      <c r="C2448" t="s"/>
-      <c r="D2448" t="s"/>
-      <c r="E2448" t="s"/>
-      <c r="F2448" t="s"/>
-      <c r="G2448" t="s"/>
-      <c r="H2448" t="s"/>
+      <c r="C2448" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="D2448" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2448" t="n">
+        <v>64.8</v>
+      </c>
+      <c r="F2448" t="n">
+        <v>39</v>
+      </c>
+      <c r="G2448" t="n">
+        <v>52.3</v>
+      </c>
+      <c r="H2448" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2449" spans="1:8">
       <c r="A2449" s="1" t="n">
@@ -68913,12 +69813,24 @@
       <c r="B2449" t="s">
         <v>1291</v>
       </c>
-      <c r="C2449" t="s"/>
-      <c r="D2449" t="s"/>
-      <c r="E2449" t="s"/>
-      <c r="F2449" t="s"/>
-      <c r="G2449" t="s"/>
-      <c r="H2449" t="s"/>
+      <c r="C2449" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="D2449" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2449" t="n">
+        <v>70.59999999999999</v>
+      </c>
+      <c r="F2449" t="n">
+        <v>70.2</v>
+      </c>
+      <c r="G2449" t="n">
+        <v>45.6</v>
+      </c>
+      <c r="H2449" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2450" spans="1:8">
       <c r="A2450" s="1" t="n">
@@ -68927,12 +69839,24 @@
       <c r="B2450" t="s">
         <v>1293</v>
       </c>
-      <c r="C2450" t="s"/>
-      <c r="D2450" t="s"/>
-      <c r="E2450" t="s"/>
-      <c r="F2450" t="s"/>
-      <c r="G2450" t="s"/>
-      <c r="H2450" t="s"/>
+      <c r="C2450" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="D2450" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2450" t="n">
+        <v>50</v>
+      </c>
+      <c r="F2450" t="n">
+        <v>39.9</v>
+      </c>
+      <c r="G2450" t="n">
+        <v>47.3</v>
+      </c>
+      <c r="H2450" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2451" spans="1:8">
       <c r="A2451" s="1" t="n">
@@ -68941,12 +69865,24 @@
       <c r="B2451" t="s">
         <v>890</v>
       </c>
-      <c r="C2451" t="s"/>
-      <c r="D2451" t="s"/>
-      <c r="E2451" t="s"/>
-      <c r="F2451" t="s"/>
-      <c r="G2451" t="s"/>
-      <c r="H2451" t="s"/>
+      <c r="C2451" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="D2451" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2451" t="n">
+        <v>28.5</v>
+      </c>
+      <c r="F2451" t="n">
+        <v>32.9</v>
+      </c>
+      <c r="G2451" t="n">
+        <v>22.1</v>
+      </c>
+      <c r="H2451" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2452" spans="1:8">
       <c r="A2452" s="1" t="n">
@@ -72205,12 +73141,24 @@
       <c r="B2577" t="s">
         <v>1292</v>
       </c>
-      <c r="C2577" t="s"/>
-      <c r="D2577" t="s"/>
-      <c r="E2577" t="s"/>
-      <c r="F2577" t="s"/>
-      <c r="G2577" t="s"/>
-      <c r="H2577" t="s"/>
+      <c r="C2577" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="D2577" t="n">
+        <v>45</v>
+      </c>
+      <c r="E2577" t="n">
+        <v>10.6</v>
+      </c>
+      <c r="F2577" t="n">
+        <v>10.2</v>
+      </c>
+      <c r="G2577" t="n">
+        <v>16.5</v>
+      </c>
+      <c r="H2577" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2578" spans="1:8">
       <c r="A2578" s="1" t="n">
@@ -72219,12 +73167,24 @@
       <c r="B2578" t="s">
         <v>201</v>
       </c>
-      <c r="C2578" t="s"/>
-      <c r="D2578" t="s"/>
-      <c r="E2578" t="s"/>
-      <c r="F2578" t="s"/>
-      <c r="G2578" t="s"/>
-      <c r="H2578" t="s"/>
+      <c r="C2578" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="D2578" t="n">
+        <v>73.5</v>
+      </c>
+      <c r="E2578" t="n">
+        <v>68.59999999999999</v>
+      </c>
+      <c r="F2578" t="n">
+        <v>67.90000000000001</v>
+      </c>
+      <c r="G2578" t="n">
+        <v>71.40000000000001</v>
+      </c>
+      <c r="H2578" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2579" spans="1:8">
       <c r="A2579" s="1" t="n">
@@ -72233,12 +73193,24 @@
       <c r="B2579" t="s">
         <v>195</v>
       </c>
-      <c r="C2579" t="s"/>
-      <c r="D2579" t="s"/>
-      <c r="E2579" t="s"/>
-      <c r="F2579" t="s"/>
-      <c r="G2579" t="s"/>
-      <c r="H2579" t="s"/>
+      <c r="C2579" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="D2579" t="n">
+        <v>89</v>
+      </c>
+      <c r="E2579" t="n">
+        <v>69.5</v>
+      </c>
+      <c r="F2579" t="n">
+        <v>68.7</v>
+      </c>
+      <c r="G2579" t="n">
+        <v>66.40000000000001</v>
+      </c>
+      <c r="H2579" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2580" spans="1:8">
       <c r="A2580" s="1" t="n">
@@ -72247,12 +73219,24 @@
       <c r="B2580" t="s">
         <v>194</v>
       </c>
-      <c r="C2580" t="s"/>
-      <c r="D2580" t="s"/>
-      <c r="E2580" t="s"/>
-      <c r="F2580" t="s"/>
-      <c r="G2580" t="s"/>
-      <c r="H2580" t="s"/>
+      <c r="C2580" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2580" t="n">
+        <v>68.3</v>
+      </c>
+      <c r="E2580" t="n">
+        <v>58</v>
+      </c>
+      <c r="F2580" t="n">
+        <v>54.4</v>
+      </c>
+      <c r="G2580" t="n">
+        <v>58.1</v>
+      </c>
+      <c r="H2580" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2581" spans="1:8">
       <c r="A2581" s="1" t="n">
@@ -72261,12 +73245,24 @@
       <c r="B2581" t="s">
         <v>890</v>
       </c>
-      <c r="C2581" t="s"/>
-      <c r="D2581" t="s"/>
-      <c r="E2581" t="s"/>
-      <c r="F2581" t="s"/>
-      <c r="G2581" t="s"/>
-      <c r="H2581" t="s"/>
+      <c r="C2581" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="D2581" t="n">
+        <v>49</v>
+      </c>
+      <c r="E2581" t="n">
+        <v>47.1</v>
+      </c>
+      <c r="F2581" t="n">
+        <v>42.2</v>
+      </c>
+      <c r="G2581" t="n">
+        <v>45</v>
+      </c>
+      <c r="H2581" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2582" spans="1:8">
       <c r="A2582" s="1" t="n">
@@ -72275,12 +73271,24 @@
       <c r="B2582" t="s">
         <v>195</v>
       </c>
-      <c r="C2582" t="s"/>
-      <c r="D2582" t="s"/>
-      <c r="E2582" t="s"/>
-      <c r="F2582" t="s"/>
-      <c r="G2582" t="s"/>
-      <c r="H2582" t="s"/>
+      <c r="C2582" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="D2582" t="n">
+        <v>52.5</v>
+      </c>
+      <c r="E2582" t="n">
+        <v>66.40000000000001</v>
+      </c>
+      <c r="F2582" t="n">
+        <v>64.90000000000001</v>
+      </c>
+      <c r="G2582" t="n">
+        <v>65.40000000000001</v>
+      </c>
+      <c r="H2582" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2583" spans="1:8">
       <c r="A2583" s="1" t="n">
@@ -72289,12 +73297,24 @@
       <c r="B2583" t="s">
         <v>197</v>
       </c>
-      <c r="C2583" t="s"/>
-      <c r="D2583" t="s"/>
-      <c r="E2583" t="s"/>
-      <c r="F2583" t="s"/>
-      <c r="G2583" t="s"/>
-      <c r="H2583" t="s"/>
+      <c r="C2583" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="D2583" t="n">
+        <v>68.5</v>
+      </c>
+      <c r="E2583" t="n">
+        <v>78.59999999999999</v>
+      </c>
+      <c r="F2583" t="n">
+        <v>87.5</v>
+      </c>
+      <c r="G2583" t="n">
+        <v>66.59999999999999</v>
+      </c>
+      <c r="H2583" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2584" spans="1:8">
       <c r="A2584" s="1" t="n">
@@ -72303,12 +73323,24 @@
       <c r="B2584" t="s">
         <v>200</v>
       </c>
-      <c r="C2584" t="s"/>
-      <c r="D2584" t="s"/>
-      <c r="E2584" t="s"/>
-      <c r="F2584" t="s"/>
-      <c r="G2584" t="s"/>
-      <c r="H2584" t="s"/>
+      <c r="C2584" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="D2584" t="n">
+        <v>73.5</v>
+      </c>
+      <c r="E2584" t="n">
+        <v>77.09999999999999</v>
+      </c>
+      <c r="F2584" t="n">
+        <v>65.8</v>
+      </c>
+      <c r="G2584" t="n">
+        <v>76.40000000000001</v>
+      </c>
+      <c r="H2584" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2585" spans="1:8">
       <c r="A2585" s="1" t="n">
@@ -72317,12 +73349,24 @@
       <c r="B2585" t="s">
         <v>194</v>
       </c>
-      <c r="C2585" t="s"/>
-      <c r="D2585" t="s"/>
-      <c r="E2585" t="s"/>
-      <c r="F2585" t="s"/>
-      <c r="G2585" t="s"/>
-      <c r="H2585" t="s"/>
+      <c r="C2585" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="D2585" t="n">
+        <v>73.5</v>
+      </c>
+      <c r="E2585" t="n">
+        <v>52.6</v>
+      </c>
+      <c r="F2585" t="n">
+        <v>47.4</v>
+      </c>
+      <c r="G2585" t="n">
+        <v>52</v>
+      </c>
+      <c r="H2585" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2586" spans="1:8">
       <c r="A2586" s="1" t="n">
@@ -72331,12 +73375,24 @@
       <c r="B2586" t="s">
         <v>197</v>
       </c>
-      <c r="C2586" t="s"/>
-      <c r="D2586" t="s"/>
-      <c r="E2586" t="s"/>
-      <c r="F2586" t="s"/>
-      <c r="G2586" t="s"/>
-      <c r="H2586" t="s"/>
+      <c r="C2586" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="D2586" t="n">
+        <v>63</v>
+      </c>
+      <c r="E2586" t="n">
+        <v>47.9</v>
+      </c>
+      <c r="F2586" t="n">
+        <v>52.9</v>
+      </c>
+      <c r="G2586" t="n">
+        <v>46.3</v>
+      </c>
+      <c r="H2586" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2587" spans="1:8">
       <c r="A2587" s="1" t="n">
@@ -72345,12 +73401,24 @@
       <c r="B2587" t="s">
         <v>195</v>
       </c>
-      <c r="C2587" t="s"/>
-      <c r="D2587" t="s"/>
-      <c r="E2587" t="s"/>
-      <c r="F2587" t="s"/>
-      <c r="G2587" t="s"/>
-      <c r="H2587" t="s"/>
+      <c r="C2587" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="D2587" t="n">
+        <v>55.6</v>
+      </c>
+      <c r="E2587" t="n">
+        <v>74.2</v>
+      </c>
+      <c r="F2587" t="n">
+        <v>60.1</v>
+      </c>
+      <c r="G2587" t="n">
+        <v>97.90000000000001</v>
+      </c>
+      <c r="H2587" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2588" spans="1:8">
       <c r="A2588" s="1" t="n">
@@ -73529,12 +74597,24 @@
       <c r="B2633" t="s">
         <v>247</v>
       </c>
-      <c r="C2633" t="s"/>
-      <c r="D2633" t="s"/>
-      <c r="E2633" t="s"/>
-      <c r="F2633" t="s"/>
-      <c r="G2633" t="s"/>
-      <c r="H2633" t="s"/>
+      <c r="C2633" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="D2633" t="n">
+        <v>110.6</v>
+      </c>
+      <c r="E2633" t="n">
+        <v>75.59999999999999</v>
+      </c>
+      <c r="F2633" t="n">
+        <v>62.4</v>
+      </c>
+      <c r="G2633" t="n">
+        <v>80.3</v>
+      </c>
+      <c r="H2633" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2634" spans="1:8">
       <c r="A2634" s="1" t="n">
@@ -73543,12 +74623,24 @@
       <c r="B2634" t="s">
         <v>194</v>
       </c>
-      <c r="C2634" t="s"/>
-      <c r="D2634" t="s"/>
-      <c r="E2634" t="s"/>
-      <c r="F2634" t="s"/>
-      <c r="G2634" t="s"/>
-      <c r="H2634" t="s"/>
+      <c r="C2634" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D2634" t="n">
+        <v>86</v>
+      </c>
+      <c r="E2634" t="n">
+        <v>95</v>
+      </c>
+      <c r="F2634" t="n">
+        <v>83.3</v>
+      </c>
+      <c r="G2634" t="n">
+        <v>93.2</v>
+      </c>
+      <c r="H2634" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2635" spans="1:8">
       <c r="A2635" s="1" t="n">
@@ -73557,12 +74649,24 @@
       <c r="B2635" t="s">
         <v>194</v>
       </c>
-      <c r="C2635" t="s"/>
-      <c r="D2635" t="s"/>
-      <c r="E2635" t="s"/>
-      <c r="F2635" t="s"/>
-      <c r="G2635" t="s"/>
-      <c r="H2635" t="s"/>
+      <c r="C2635" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="D2635" t="n">
+        <v>92.2</v>
+      </c>
+      <c r="E2635" t="n">
+        <v>83.2</v>
+      </c>
+      <c r="F2635" t="n">
+        <v>98.7</v>
+      </c>
+      <c r="G2635" t="n">
+        <v>74.09999999999999</v>
+      </c>
+      <c r="H2635" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2636" spans="1:8">
       <c r="A2636" s="1" t="n">
@@ -73571,12 +74675,24 @@
       <c r="B2636" t="s">
         <v>195</v>
       </c>
-      <c r="C2636" t="s"/>
-      <c r="D2636" t="s"/>
-      <c r="E2636" t="s"/>
-      <c r="F2636" t="s"/>
-      <c r="G2636" t="s"/>
-      <c r="H2636" t="s"/>
+      <c r="C2636" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="D2636" t="n">
+        <v>62.2</v>
+      </c>
+      <c r="E2636" t="n">
+        <v>68.90000000000001</v>
+      </c>
+      <c r="F2636" t="n">
+        <v>75.5</v>
+      </c>
+      <c r="G2636" t="n">
+        <v>49.2</v>
+      </c>
+      <c r="H2636" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2637" spans="1:8">
       <c r="A2637" s="1" t="n">
@@ -73585,12 +74701,24 @@
       <c r="B2637" t="s">
         <v>197</v>
       </c>
-      <c r="C2637" t="s"/>
-      <c r="D2637" t="s"/>
-      <c r="E2637" t="s"/>
-      <c r="F2637" t="s"/>
-      <c r="G2637" t="s"/>
-      <c r="H2637" t="s"/>
+      <c r="C2637" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="D2637" t="n">
+        <v>73.7</v>
+      </c>
+      <c r="E2637" t="n">
+        <v>85.3</v>
+      </c>
+      <c r="F2637" t="n">
+        <v>78.09999999999999</v>
+      </c>
+      <c r="G2637" t="n">
+        <v>89.90000000000001</v>
+      </c>
+      <c r="H2637" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2638" spans="1:8">
       <c r="A2638" s="1" t="n">
@@ -73599,12 +74727,24 @@
       <c r="B2638" t="s">
         <v>200</v>
       </c>
-      <c r="C2638" t="s"/>
-      <c r="D2638" t="s"/>
-      <c r="E2638" t="s"/>
-      <c r="F2638" t="s"/>
-      <c r="G2638" t="s"/>
-      <c r="H2638" t="s"/>
+      <c r="C2638" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="D2638" t="n">
+        <v>61.5</v>
+      </c>
+      <c r="E2638" t="n">
+        <v>87.59999999999999</v>
+      </c>
+      <c r="F2638" t="n">
+        <v>88.8</v>
+      </c>
+      <c r="G2638" t="n">
+        <v>72.40000000000001</v>
+      </c>
+      <c r="H2638" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2639" spans="1:8">
       <c r="A2639" s="1" t="n">
@@ -73613,12 +74753,24 @@
       <c r="B2639" t="s">
         <v>1293</v>
       </c>
-      <c r="C2639" t="s"/>
-      <c r="D2639" t="s"/>
-      <c r="E2639" t="s"/>
-      <c r="F2639" t="s"/>
-      <c r="G2639" t="s"/>
-      <c r="H2639" t="s"/>
+      <c r="C2639" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="D2639" t="n">
+        <v>55.2</v>
+      </c>
+      <c r="E2639" t="n">
+        <v>30.7</v>
+      </c>
+      <c r="F2639" t="n">
+        <v>35.4</v>
+      </c>
+      <c r="G2639" t="n">
+        <v>22.9</v>
+      </c>
+      <c r="H2639" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2640" spans="1:8">
       <c r="A2640" s="1" t="n">
@@ -73627,12 +74779,24 @@
       <c r="B2640" t="s">
         <v>1293</v>
       </c>
-      <c r="C2640" t="s"/>
-      <c r="D2640" t="s"/>
-      <c r="E2640" t="s"/>
-      <c r="F2640" t="s"/>
-      <c r="G2640" t="s"/>
-      <c r="H2640" t="s"/>
+      <c r="C2640" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2640" t="n">
+        <v>55.5</v>
+      </c>
+      <c r="E2640" t="n">
+        <v>94.40000000000001</v>
+      </c>
+      <c r="F2640" t="n">
+        <v>28.9</v>
+      </c>
+      <c r="G2640" t="n">
+        <v>41</v>
+      </c>
+      <c r="H2640" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2641" spans="1:8">
       <c r="A2641" s="1" t="n">
@@ -73641,12 +74805,24 @@
       <c r="B2641" t="s">
         <v>194</v>
       </c>
-      <c r="C2641" t="s"/>
-      <c r="D2641" t="s"/>
-      <c r="E2641" t="s"/>
-      <c r="F2641" t="s"/>
-      <c r="G2641" t="s"/>
-      <c r="H2641" t="s"/>
+      <c r="C2641" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="D2641" t="n">
+        <v>70</v>
+      </c>
+      <c r="E2641" t="n">
+        <v>69.7</v>
+      </c>
+      <c r="F2641" t="n">
+        <v>91.40000000000001</v>
+      </c>
+      <c r="G2641" t="n">
+        <v>55.9</v>
+      </c>
+      <c r="H2641" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2642" spans="1:8">
       <c r="A2642" s="1" t="n">
@@ -73655,12 +74831,24 @@
       <c r="B2642" t="s">
         <v>194</v>
       </c>
-      <c r="C2642" t="s"/>
-      <c r="D2642" t="s"/>
-      <c r="E2642" t="s"/>
-      <c r="F2642" t="s"/>
-      <c r="G2642" t="s"/>
-      <c r="H2642" t="s"/>
+      <c r="C2642" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="D2642" t="n">
+        <v>63.6</v>
+      </c>
+      <c r="E2642" t="n">
+        <v>76.09999999999999</v>
+      </c>
+      <c r="F2642" t="n">
+        <v>84.90000000000001</v>
+      </c>
+      <c r="G2642" t="n">
+        <v>66.40000000000001</v>
+      </c>
+      <c r="H2642" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2643" spans="1:8">
       <c r="A2643" s="1" t="n">
@@ -73669,12 +74857,24 @@
       <c r="B2643" t="s">
         <v>200</v>
       </c>
-      <c r="C2643" t="s"/>
-      <c r="D2643" t="s"/>
-      <c r="E2643" t="s"/>
-      <c r="F2643" t="s"/>
-      <c r="G2643" t="s"/>
-      <c r="H2643" t="s"/>
+      <c r="C2643" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="D2643" t="n">
+        <v>51.8</v>
+      </c>
+      <c r="E2643" t="n">
+        <v>55.1</v>
+      </c>
+      <c r="F2643" t="n">
+        <v>61</v>
+      </c>
+      <c r="G2643" t="n">
+        <v>44.5</v>
+      </c>
+      <c r="H2643" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2644" spans="1:8">
       <c r="A2644" s="1" t="n">
@@ -73683,12 +74883,24 @@
       <c r="B2644" t="s">
         <v>194</v>
       </c>
-      <c r="C2644" t="s"/>
-      <c r="D2644" t="s"/>
-      <c r="E2644" t="s"/>
-      <c r="F2644" t="s"/>
-      <c r="G2644" t="s"/>
-      <c r="H2644" t="s"/>
+      <c r="C2644" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="D2644" t="n">
+        <v>62.2</v>
+      </c>
+      <c r="E2644" t="n">
+        <v>72.3</v>
+      </c>
+      <c r="F2644" t="n">
+        <v>79.5</v>
+      </c>
+      <c r="G2644" t="n">
+        <v>69.09999999999999</v>
+      </c>
+      <c r="H2644" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2645" spans="1:8">
       <c r="A2645" s="1" t="n">
@@ -73697,12 +74909,24 @@
       <c r="B2645" t="s">
         <v>200</v>
       </c>
-      <c r="C2645" t="s"/>
-      <c r="D2645" t="s"/>
-      <c r="E2645" t="s"/>
-      <c r="F2645" t="s"/>
-      <c r="G2645" t="s"/>
-      <c r="H2645" t="s"/>
+      <c r="C2645" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="D2645" t="n">
+        <v>99.5</v>
+      </c>
+      <c r="E2645" t="n">
+        <v>108.2</v>
+      </c>
+      <c r="F2645" t="n">
+        <v>98.5</v>
+      </c>
+      <c r="G2645" t="n">
+        <v>123.1</v>
+      </c>
+      <c r="H2645" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2646" spans="1:8">
       <c r="A2646" s="1" t="n">
@@ -73711,12 +74935,24 @@
       <c r="B2646" t="s">
         <v>194</v>
       </c>
-      <c r="C2646" t="s"/>
-      <c r="D2646" t="s"/>
-      <c r="E2646" t="s"/>
-      <c r="F2646" t="s"/>
-      <c r="G2646" t="s"/>
-      <c r="H2646" t="s"/>
+      <c r="C2646" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="D2646" t="n">
+        <v>62.2</v>
+      </c>
+      <c r="E2646" t="n">
+        <v>57.2</v>
+      </c>
+      <c r="F2646" t="n">
+        <v>46.9</v>
+      </c>
+      <c r="G2646" t="n">
+        <v>52.4</v>
+      </c>
+      <c r="H2646" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2647" spans="1:8">
       <c r="A2647" s="1" t="n">
@@ -73725,12 +74961,24 @@
       <c r="B2647" t="s">
         <v>201</v>
       </c>
-      <c r="C2647" t="s"/>
-      <c r="D2647" t="s"/>
-      <c r="E2647" t="s"/>
-      <c r="F2647" t="s"/>
-      <c r="G2647" t="s"/>
-      <c r="H2647" t="s"/>
+      <c r="C2647" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="D2647" t="n">
+        <v>81</v>
+      </c>
+      <c r="E2647" t="n">
+        <v>80.09999999999999</v>
+      </c>
+      <c r="F2647" t="n">
+        <v>76.2</v>
+      </c>
+      <c r="G2647" t="n">
+        <v>71.09999999999999</v>
+      </c>
+      <c r="H2647" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2648" spans="1:8">
       <c r="A2648" s="1" t="n">
@@ -73739,12 +74987,24 @@
       <c r="B2648" t="s">
         <v>194</v>
       </c>
-      <c r="C2648" t="s"/>
-      <c r="D2648" t="s"/>
-      <c r="E2648" t="s"/>
-      <c r="F2648" t="s"/>
-      <c r="G2648" t="s"/>
-      <c r="H2648" t="s"/>
+      <c r="C2648" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="D2648" t="n">
+        <v>87.09999999999999</v>
+      </c>
+      <c r="E2648" t="n">
+        <v>85.8</v>
+      </c>
+      <c r="F2648" t="n">
+        <v>61.1</v>
+      </c>
+      <c r="G2648" t="n">
+        <v>107.5</v>
+      </c>
+      <c r="H2648" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2649" spans="1:8">
       <c r="A2649" s="1" t="n">
@@ -73753,12 +75013,24 @@
       <c r="B2649" t="s">
         <v>1292</v>
       </c>
-      <c r="C2649" t="s"/>
-      <c r="D2649" t="s"/>
-      <c r="E2649" t="s"/>
-      <c r="F2649" t="s"/>
-      <c r="G2649" t="s"/>
-      <c r="H2649" t="s"/>
+      <c r="C2649" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="D2649" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="E2649" t="n">
+        <v>13.9</v>
+      </c>
+      <c r="F2649" t="n">
+        <v>17.5</v>
+      </c>
+      <c r="G2649" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2649" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2650" spans="1:8">
       <c r="A2650" s="1" t="n">
@@ -73767,12 +75039,24 @@
       <c r="B2650" t="s">
         <v>247</v>
       </c>
-      <c r="C2650" t="s"/>
-      <c r="D2650" t="s"/>
-      <c r="E2650" t="s"/>
-      <c r="F2650" t="s"/>
-      <c r="G2650" t="s"/>
-      <c r="H2650" t="s"/>
+      <c r="C2650" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="D2650" t="n">
+        <v>124.4</v>
+      </c>
+      <c r="E2650" t="n">
+        <v>107.2</v>
+      </c>
+      <c r="F2650" t="n">
+        <v>103.3</v>
+      </c>
+      <c r="G2650" t="n">
+        <v>117.1</v>
+      </c>
+      <c r="H2650" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2651" spans="1:8">
       <c r="A2651" s="1" t="n">
@@ -73781,12 +75065,24 @@
       <c r="B2651" t="s">
         <v>201</v>
       </c>
-      <c r="C2651" t="s"/>
-      <c r="D2651" t="s"/>
-      <c r="E2651" t="s"/>
-      <c r="F2651" t="s"/>
-      <c r="G2651" t="s"/>
-      <c r="H2651" t="s"/>
+      <c r="C2651" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="D2651" t="n">
+        <v>87.09999999999999</v>
+      </c>
+      <c r="E2651" t="n">
+        <v>76.59999999999999</v>
+      </c>
+      <c r="F2651" t="n">
+        <v>73.40000000000001</v>
+      </c>
+      <c r="G2651" t="n">
+        <v>72.09999999999999</v>
+      </c>
+      <c r="H2651" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2652" spans="1:8">
       <c r="A2652" s="1" t="n">
@@ -73795,12 +75091,24 @@
       <c r="B2652" t="s">
         <v>1293</v>
       </c>
-      <c r="C2652" t="s"/>
-      <c r="D2652" t="s"/>
-      <c r="E2652" t="s"/>
-      <c r="F2652" t="s"/>
-      <c r="G2652" t="s"/>
-      <c r="H2652" t="s"/>
+      <c r="C2652" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D2652" t="n">
+        <v>58.7</v>
+      </c>
+      <c r="E2652" t="n">
+        <v>155.1</v>
+      </c>
+      <c r="F2652" t="n">
+        <v>49.4</v>
+      </c>
+      <c r="G2652" t="n">
+        <v>54.2</v>
+      </c>
+      <c r="H2652" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2653" spans="1:8">
       <c r="A2653" s="1" t="n">
@@ -73809,12 +75117,24 @@
       <c r="B2653" t="s">
         <v>200</v>
       </c>
-      <c r="C2653" t="s"/>
-      <c r="D2653" t="s"/>
-      <c r="E2653" t="s"/>
-      <c r="F2653" t="s"/>
-      <c r="G2653" t="s"/>
-      <c r="H2653" t="s"/>
+      <c r="C2653" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="D2653" t="n">
+        <v>74.59999999999999</v>
+      </c>
+      <c r="E2653" t="n">
+        <v>95.7</v>
+      </c>
+      <c r="F2653" t="n">
+        <v>77.40000000000001</v>
+      </c>
+      <c r="G2653" t="n">
+        <v>121.5</v>
+      </c>
+      <c r="H2653" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2654" spans="1:8">
       <c r="A2654" s="1" t="n">
@@ -73823,12 +75143,24 @@
       <c r="B2654" t="s">
         <v>195</v>
       </c>
-      <c r="C2654" t="s"/>
-      <c r="D2654" t="s"/>
-      <c r="E2654" t="s"/>
-      <c r="F2654" t="s"/>
-      <c r="G2654" t="s"/>
-      <c r="H2654" t="s"/>
+      <c r="C2654" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="D2654" t="n">
+        <v>74.59999999999999</v>
+      </c>
+      <c r="E2654" t="n">
+        <v>92.5</v>
+      </c>
+      <c r="F2654" t="n">
+        <v>73</v>
+      </c>
+      <c r="G2654" t="n">
+        <v>123.8</v>
+      </c>
+      <c r="H2654" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2655" spans="1:8">
       <c r="A2655" s="1" t="n">
@@ -73837,12 +75169,24 @@
       <c r="B2655" t="s">
         <v>200</v>
       </c>
-      <c r="C2655" t="s"/>
-      <c r="D2655" t="s"/>
-      <c r="E2655" t="s"/>
-      <c r="F2655" t="s"/>
-      <c r="G2655" t="s"/>
-      <c r="H2655" t="s"/>
+      <c r="C2655" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="D2655" t="n">
+        <v>111.9</v>
+      </c>
+      <c r="E2655" t="n">
+        <v>112.1</v>
+      </c>
+      <c r="F2655" t="n">
+        <v>102.4</v>
+      </c>
+      <c r="G2655" t="n">
+        <v>167.8</v>
+      </c>
+      <c r="H2655" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2656" spans="1:8">
       <c r="A2656" s="1" t="n">
@@ -76737,12 +78081,24 @@
       <c r="B2767" t="s">
         <v>200</v>
       </c>
-      <c r="C2767" t="s"/>
-      <c r="D2767" t="s"/>
-      <c r="E2767" t="s"/>
-      <c r="F2767" t="s"/>
-      <c r="G2767" t="s"/>
-      <c r="H2767" t="s"/>
+      <c r="C2767" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="D2767" t="n">
+        <v>101.9</v>
+      </c>
+      <c r="E2767" t="n">
+        <v>99.09999999999999</v>
+      </c>
+      <c r="F2767" t="n">
+        <v>86.3</v>
+      </c>
+      <c r="G2767" t="n">
+        <v>80.2</v>
+      </c>
+      <c r="H2767" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2768" spans="1:8">
       <c r="A2768" s="1" t="n">
@@ -76751,12 +78107,24 @@
       <c r="B2768" t="s">
         <v>195</v>
       </c>
-      <c r="C2768" t="s"/>
-      <c r="D2768" t="s"/>
-      <c r="E2768" t="s"/>
-      <c r="F2768" t="s"/>
-      <c r="G2768" t="s"/>
-      <c r="H2768" t="s"/>
+      <c r="C2768" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="D2768" t="n">
+        <v>101.6</v>
+      </c>
+      <c r="E2768" t="n">
+        <v>76.09999999999999</v>
+      </c>
+      <c r="F2768" t="n">
+        <v>58.5</v>
+      </c>
+      <c r="G2768" t="n">
+        <v>90.8</v>
+      </c>
+      <c r="H2768" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2769" spans="1:8">
       <c r="A2769" s="1" t="n">
@@ -76765,12 +78133,24 @@
       <c r="B2769" t="s">
         <v>200</v>
       </c>
-      <c r="C2769" t="s"/>
-      <c r="D2769" t="s"/>
-      <c r="E2769" t="s"/>
-      <c r="F2769" t="s"/>
-      <c r="G2769" t="s"/>
-      <c r="H2769" t="s"/>
+      <c r="C2769" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="D2769" t="n">
+        <v>101.9</v>
+      </c>
+      <c r="E2769" t="n">
+        <v>99.7</v>
+      </c>
+      <c r="F2769" t="n">
+        <v>80.90000000000001</v>
+      </c>
+      <c r="G2769" t="n">
+        <v>93.2</v>
+      </c>
+      <c r="H2769" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2770" spans="1:8">
       <c r="A2770" s="1" t="n">
@@ -76779,12 +78159,24 @@
       <c r="B2770" t="s">
         <v>195</v>
       </c>
-      <c r="C2770" t="s"/>
-      <c r="D2770" t="s"/>
-      <c r="E2770" t="s"/>
-      <c r="F2770" t="s"/>
-      <c r="G2770" t="s"/>
-      <c r="H2770" t="s"/>
+      <c r="C2770" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="D2770" t="n">
+        <v>101.9</v>
+      </c>
+      <c r="E2770" t="n">
+        <v>100.6</v>
+      </c>
+      <c r="F2770" t="n">
+        <v>85.3</v>
+      </c>
+      <c r="G2770" t="n">
+        <v>93</v>
+      </c>
+      <c r="H2770" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2771" spans="1:8">
       <c r="A2771" s="1" t="n">
@@ -76793,12 +78185,24 @@
       <c r="B2771" t="s">
         <v>201</v>
       </c>
-      <c r="C2771" t="s"/>
-      <c r="D2771" t="s"/>
-      <c r="E2771" t="s"/>
-      <c r="F2771" t="s"/>
-      <c r="G2771" t="s"/>
-      <c r="H2771" t="s"/>
+      <c r="C2771" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="D2771" t="n">
+        <v>101.9</v>
+      </c>
+      <c r="E2771" t="n">
+        <v>86.3</v>
+      </c>
+      <c r="F2771" t="n">
+        <v>65.59999999999999</v>
+      </c>
+      <c r="G2771" t="n">
+        <v>82.3</v>
+      </c>
+      <c r="H2771" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2772" spans="1:8">
       <c r="A2772" s="1" t="n">
@@ -76807,12 +78211,24 @@
       <c r="B2772" t="s">
         <v>201</v>
       </c>
-      <c r="C2772" t="s"/>
-      <c r="D2772" t="s"/>
-      <c r="E2772" t="s"/>
-      <c r="F2772" t="s"/>
-      <c r="G2772" t="s"/>
-      <c r="H2772" t="s"/>
+      <c r="C2772" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="D2772" t="n">
+        <v>83.8</v>
+      </c>
+      <c r="E2772" t="n">
+        <v>70.2</v>
+      </c>
+      <c r="F2772" t="n">
+        <v>72.8</v>
+      </c>
+      <c r="G2772" t="n">
+        <v>64.40000000000001</v>
+      </c>
+      <c r="H2772" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2773" spans="1:8">
       <c r="A2773" s="1" t="n">
@@ -79187,12 +80603,24 @@
       <c r="B2864" t="s">
         <v>200</v>
       </c>
-      <c r="C2864" t="s"/>
-      <c r="D2864" t="s"/>
-      <c r="E2864" t="s"/>
-      <c r="F2864" t="s"/>
-      <c r="G2864" t="s"/>
-      <c r="H2864" t="s"/>
+      <c r="C2864" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="D2864" t="n">
+        <v>98.59999999999999</v>
+      </c>
+      <c r="E2864" t="n">
+        <v>25.2</v>
+      </c>
+      <c r="F2864" t="n">
+        <v>23.9</v>
+      </c>
+      <c r="G2864" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="H2864" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2865" spans="1:8">
       <c r="A2865" s="1" t="n">
@@ -79201,12 +80629,24 @@
       <c r="B2865" t="s">
         <v>195</v>
       </c>
-      <c r="C2865" t="s"/>
-      <c r="D2865" t="s"/>
-      <c r="E2865" t="s"/>
-      <c r="F2865" t="s"/>
-      <c r="G2865" t="s"/>
-      <c r="H2865" t="s"/>
+      <c r="C2865" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="D2865" t="n">
+        <v>75.2</v>
+      </c>
+      <c r="E2865" t="n">
+        <v>23.9</v>
+      </c>
+      <c r="F2865" t="n">
+        <v>17.1</v>
+      </c>
+      <c r="G2865" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2865" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2866" spans="1:8">
       <c r="A2866" s="1" t="n">
@@ -79215,12 +80655,24 @@
       <c r="B2866" t="s">
         <v>195</v>
       </c>
-      <c r="C2866" t="s"/>
-      <c r="D2866" t="s"/>
-      <c r="E2866" t="s"/>
-      <c r="F2866" t="s"/>
-      <c r="G2866" t="s"/>
-      <c r="H2866" t="s"/>
+      <c r="C2866" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="D2866" t="n">
+        <v>100.1</v>
+      </c>
+      <c r="E2866" t="n">
+        <v>99.09999999999999</v>
+      </c>
+      <c r="F2866" t="n">
+        <v>96.59999999999999</v>
+      </c>
+      <c r="G2866" t="n">
+        <v>87.90000000000001</v>
+      </c>
+      <c r="H2866" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2867" spans="1:8">
       <c r="A2867" s="1" t="n">
@@ -79229,12 +80681,24 @@
       <c r="B2867" t="s">
         <v>195</v>
       </c>
-      <c r="C2867" t="s"/>
-      <c r="D2867" t="s"/>
-      <c r="E2867" t="s"/>
-      <c r="F2867" t="s"/>
-      <c r="G2867" t="s"/>
-      <c r="H2867" t="s"/>
+      <c r="C2867" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="D2867" t="n">
+        <v>87.7</v>
+      </c>
+      <c r="E2867" t="n">
+        <v>53.8</v>
+      </c>
+      <c r="F2867" t="n">
+        <v>44.4</v>
+      </c>
+      <c r="G2867" t="n">
+        <v>74.59999999999999</v>
+      </c>
+      <c r="H2867" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2868" spans="1:8">
       <c r="A2868" s="1" t="n">
@@ -79243,12 +80707,24 @@
       <c r="B2868" t="s">
         <v>195</v>
       </c>
-      <c r="C2868" t="s"/>
-      <c r="D2868" t="s"/>
-      <c r="E2868" t="s"/>
-      <c r="F2868" t="s"/>
-      <c r="G2868" t="s"/>
-      <c r="H2868" t="s"/>
+      <c r="C2868" t="n">
+        <v>4</v>
+      </c>
+      <c r="D2868" t="n">
+        <v>75.2</v>
+      </c>
+      <c r="E2868" t="n">
+        <v>78.5</v>
+      </c>
+      <c r="F2868" t="n">
+        <v>94.7</v>
+      </c>
+      <c r="G2868" t="n">
+        <v>67.59999999999999</v>
+      </c>
+      <c r="H2868" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2869" spans="1:8">
       <c r="A2869" s="1" t="n">
@@ -80817,12 +82293,24 @@
       <c r="B2929" t="s">
         <v>200</v>
       </c>
-      <c r="C2929" t="s"/>
-      <c r="D2929" t="s"/>
-      <c r="E2929" t="s"/>
-      <c r="F2929" t="s"/>
-      <c r="G2929" t="s"/>
-      <c r="H2929" t="s"/>
+      <c r="C2929" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="D2929" t="n">
+        <v>112.3</v>
+      </c>
+      <c r="E2929" t="n">
+        <v>92.90000000000001</v>
+      </c>
+      <c r="F2929" t="n">
+        <v>76.59999999999999</v>
+      </c>
+      <c r="G2929" t="n">
+        <v>103</v>
+      </c>
+      <c r="H2929" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2930" spans="1:8">
       <c r="A2930" s="1" t="n">
@@ -80831,12 +82319,24 @@
       <c r="B2930" t="s">
         <v>194</v>
       </c>
-      <c r="C2930" t="s"/>
-      <c r="D2930" t="s"/>
-      <c r="E2930" t="s"/>
-      <c r="F2930" t="s"/>
-      <c r="G2930" t="s"/>
-      <c r="H2930" t="s"/>
+      <c r="C2930" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="D2930" t="n">
+        <v>99.8</v>
+      </c>
+      <c r="E2930" t="n">
+        <v>100</v>
+      </c>
+      <c r="F2930" t="n">
+        <v>97.40000000000001</v>
+      </c>
+      <c r="G2930" t="n">
+        <v>97.7</v>
+      </c>
+      <c r="H2930" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2931" spans="1:8">
       <c r="A2931" s="1" t="n">
@@ -80845,12 +82345,24 @@
       <c r="B2931" t="s">
         <v>247</v>
       </c>
-      <c r="C2931" t="s"/>
-      <c r="D2931" t="s"/>
-      <c r="E2931" t="s"/>
-      <c r="F2931" t="s"/>
-      <c r="G2931" t="s"/>
-      <c r="H2931" t="s"/>
+      <c r="C2931" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="D2931" t="n">
+        <v>74.90000000000001</v>
+      </c>
+      <c r="E2931" t="n">
+        <v>69.90000000000001</v>
+      </c>
+      <c r="F2931" t="n">
+        <v>54.1</v>
+      </c>
+      <c r="G2931" t="n">
+        <v>68.5</v>
+      </c>
+      <c r="H2931" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2932" spans="1:8">
       <c r="A2932" s="1" t="n">
@@ -80859,12 +82371,24 @@
       <c r="B2932" t="s">
         <v>201</v>
       </c>
-      <c r="C2932" t="s"/>
-      <c r="D2932" t="s"/>
-      <c r="E2932" t="s"/>
-      <c r="F2932" t="s"/>
-      <c r="G2932" t="s"/>
-      <c r="H2932" t="s"/>
+      <c r="C2932" t="n">
+        <v>5</v>
+      </c>
+      <c r="D2932" t="n">
+        <v>87.3</v>
+      </c>
+      <c r="E2932" t="n">
+        <v>112.5</v>
+      </c>
+      <c r="F2932" t="n">
+        <v>93</v>
+      </c>
+      <c r="G2932" t="n">
+        <v>107.6</v>
+      </c>
+      <c r="H2932" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2933" spans="1:8">
       <c r="A2933" s="1" t="n">
@@ -80873,12 +82397,24 @@
       <c r="B2933" t="s">
         <v>247</v>
       </c>
-      <c r="C2933" t="s"/>
-      <c r="D2933" t="s"/>
-      <c r="E2933" t="s"/>
-      <c r="F2933" t="s"/>
-      <c r="G2933" t="s"/>
-      <c r="H2933" t="s"/>
+      <c r="C2933" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="D2933" t="n">
+        <v>81.09999999999999</v>
+      </c>
+      <c r="E2933" t="n">
+        <v>98.2</v>
+      </c>
+      <c r="F2933" t="n">
+        <v>90</v>
+      </c>
+      <c r="G2933" t="n">
+        <v>85.59999999999999</v>
+      </c>
+      <c r="H2933" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2934" spans="1:8">
       <c r="A2934" s="1" t="n">
@@ -83019,12 +84555,24 @@
       <c r="B3016" t="s">
         <v>200</v>
       </c>
-      <c r="C3016" t="s"/>
-      <c r="D3016" t="s"/>
-      <c r="E3016" t="s"/>
-      <c r="F3016" t="s"/>
-      <c r="G3016" t="s"/>
-      <c r="H3016" t="s"/>
+      <c r="C3016" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="D3016" t="n">
+        <v>76.40000000000001</v>
+      </c>
+      <c r="E3016" t="n">
+        <v>36.8</v>
+      </c>
+      <c r="F3016" t="n">
+        <v>25.8</v>
+      </c>
+      <c r="G3016" t="n">
+        <v>38.1</v>
+      </c>
+      <c r="H3016" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3017" spans="1:8">
       <c r="A3017" s="1" t="n">
@@ -83033,12 +84581,24 @@
       <c r="B3017" t="s">
         <v>890</v>
       </c>
-      <c r="C3017" t="s"/>
-      <c r="D3017" t="s"/>
-      <c r="E3017" t="s"/>
-      <c r="F3017" t="s"/>
-      <c r="G3017" t="s"/>
-      <c r="H3017" t="s"/>
+      <c r="C3017" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="D3017" t="n">
+        <v>59.6</v>
+      </c>
+      <c r="E3017" t="n">
+        <v>14.7</v>
+      </c>
+      <c r="F3017" t="n">
+        <v>15.7</v>
+      </c>
+      <c r="G3017" t="n">
+        <v>26.6</v>
+      </c>
+      <c r="H3017" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3018" spans="1:8">
       <c r="A3018" s="1" t="n">
@@ -83047,12 +84607,24 @@
       <c r="B3018" t="s">
         <v>247</v>
       </c>
-      <c r="C3018" t="s"/>
-      <c r="D3018" t="s"/>
-      <c r="E3018" t="s"/>
-      <c r="F3018" t="s"/>
-      <c r="G3018" t="s"/>
-      <c r="H3018" t="s"/>
+      <c r="C3018" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="D3018" t="n">
+        <v>82.59999999999999</v>
+      </c>
+      <c r="E3018" t="n">
+        <v>98.3</v>
+      </c>
+      <c r="F3018" t="n">
+        <v>85.2</v>
+      </c>
+      <c r="G3018" t="n">
+        <v>108.3</v>
+      </c>
+      <c r="H3018" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3019" spans="1:8">
       <c r="A3019" s="1" t="n">
@@ -86311,12 +87883,24 @@
       <c r="B3144" t="s">
         <v>197</v>
       </c>
-      <c r="C3144" t="s"/>
-      <c r="D3144" t="s"/>
-      <c r="E3144" t="s"/>
-      <c r="F3144" t="s"/>
-      <c r="G3144" t="s"/>
-      <c r="H3144" t="s"/>
+      <c r="C3144" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="D3144" t="n">
+        <v>101.6</v>
+      </c>
+      <c r="E3144" t="n">
+        <v>48.8</v>
+      </c>
+      <c r="F3144" t="n">
+        <v>43</v>
+      </c>
+      <c r="G3144" t="n">
+        <v>54.1</v>
+      </c>
+      <c r="H3144" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3145" spans="1:8">
       <c r="A3145" s="1" t="n">
@@ -86325,12 +87909,24 @@
       <c r="B3145" t="s">
         <v>195</v>
       </c>
-      <c r="C3145" t="s"/>
-      <c r="D3145" t="s"/>
-      <c r="E3145" t="s"/>
-      <c r="F3145" t="s"/>
-      <c r="G3145" t="s"/>
-      <c r="H3145" t="s"/>
+      <c r="C3145" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="D3145" t="n">
+        <v>95.2</v>
+      </c>
+      <c r="E3145" t="n">
+        <v>35.6</v>
+      </c>
+      <c r="F3145" t="n">
+        <v>24.4</v>
+      </c>
+      <c r="G3145" t="n">
+        <v>41.5</v>
+      </c>
+      <c r="H3145" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3146" spans="1:8">
       <c r="A3146" s="1" t="n">
@@ -86339,12 +87935,24 @@
       <c r="B3146" t="s">
         <v>195</v>
       </c>
-      <c r="C3146" t="s"/>
-      <c r="D3146" t="s"/>
-      <c r="E3146" t="s"/>
-      <c r="F3146" t="s"/>
-      <c r="G3146" t="s"/>
-      <c r="H3146" t="s"/>
+      <c r="C3146" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="D3146" t="n">
+        <v>77.59999999999999</v>
+      </c>
+      <c r="E3146" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="F3146" t="n">
+        <v>16</v>
+      </c>
+      <c r="G3146" t="n">
+        <v>50.6</v>
+      </c>
+      <c r="H3146" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3147" spans="1:8">
       <c r="A3147" s="1" t="n">
@@ -86353,12 +87961,24 @@
       <c r="B3147" t="s">
         <v>195</v>
       </c>
-      <c r="C3147" t="s"/>
-      <c r="D3147" t="s"/>
-      <c r="E3147" t="s"/>
-      <c r="F3147" t="s"/>
-      <c r="G3147" t="s"/>
-      <c r="H3147" t="s"/>
+      <c r="C3147" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="D3147" t="n">
+        <v>90.3</v>
+      </c>
+      <c r="E3147" t="n">
+        <v>85</v>
+      </c>
+      <c r="F3147" t="n">
+        <v>91.90000000000001</v>
+      </c>
+      <c r="G3147" t="n">
+        <v>82.8</v>
+      </c>
+      <c r="H3147" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3148" spans="1:8">
       <c r="A3148" s="1" t="n">
@@ -86367,12 +87987,24 @@
       <c r="B3148" t="s">
         <v>247</v>
       </c>
-      <c r="C3148" t="s"/>
-      <c r="D3148" t="s"/>
-      <c r="E3148" t="s"/>
-      <c r="F3148" t="s"/>
-      <c r="G3148" t="s"/>
-      <c r="H3148" t="s"/>
+      <c r="C3148" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="D3148" t="n">
+        <v>103.1</v>
+      </c>
+      <c r="E3148" t="n">
+        <v>50.4</v>
+      </c>
+      <c r="F3148" t="n">
+        <v>15.7</v>
+      </c>
+      <c r="G3148" t="n">
+        <v>82.3</v>
+      </c>
+      <c r="H3148" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3149" spans="1:8">
       <c r="A3149" s="1" t="n">
@@ -86381,12 +88013,24 @@
       <c r="B3149" t="s">
         <v>200</v>
       </c>
-      <c r="C3149" t="s"/>
-      <c r="D3149" t="s"/>
-      <c r="E3149" t="s"/>
-      <c r="F3149" t="s"/>
-      <c r="G3149" t="s"/>
-      <c r="H3149" t="s"/>
+      <c r="C3149" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="D3149" t="n">
+        <v>96.3</v>
+      </c>
+      <c r="E3149" t="n">
+        <v>77.5</v>
+      </c>
+      <c r="F3149" t="n">
+        <v>87.3</v>
+      </c>
+      <c r="G3149" t="n">
+        <v>70.59999999999999</v>
+      </c>
+      <c r="H3149" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3150" spans="1:8">
       <c r="A3150" s="1" t="n">
@@ -87643,12 +89287,24 @@
       <c r="B3198" t="s">
         <v>247</v>
       </c>
-      <c r="C3198" t="s"/>
-      <c r="D3198" t="s"/>
-      <c r="E3198" t="s"/>
-      <c r="F3198" t="s"/>
-      <c r="G3198" t="s"/>
-      <c r="H3198" t="s"/>
+      <c r="C3198" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="D3198" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3198" t="n">
+        <v>7.4</v>
+      </c>
+      <c r="F3198" t="n">
+        <v>5</v>
+      </c>
+      <c r="G3198" t="n">
+        <v>21.7</v>
+      </c>
+      <c r="H3198" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3199" spans="1:8">
       <c r="A3199" s="1" t="n">
@@ -87657,12 +89313,24 @@
       <c r="B3199" t="s">
         <v>197</v>
       </c>
-      <c r="C3199" t="s"/>
-      <c r="D3199" t="s"/>
-      <c r="E3199" t="s"/>
-      <c r="F3199" t="s"/>
-      <c r="G3199" t="s"/>
-      <c r="H3199" t="s"/>
+      <c r="C3199" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="D3199" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3199" t="n">
+        <v>47.3</v>
+      </c>
+      <c r="F3199" t="n">
+        <v>72.5</v>
+      </c>
+      <c r="G3199" t="n">
+        <v>44.4</v>
+      </c>
+      <c r="H3199" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3200" spans="1:8">
       <c r="A3200" s="1" t="n">
@@ -87671,12 +89339,24 @@
       <c r="B3200" t="s">
         <v>247</v>
       </c>
-      <c r="C3200" t="s"/>
-      <c r="D3200" t="s"/>
-      <c r="E3200" t="s"/>
-      <c r="F3200" t="s"/>
-      <c r="G3200" t="s"/>
-      <c r="H3200" t="s"/>
+      <c r="C3200" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D3200" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3200" t="n">
+        <v>13.8</v>
+      </c>
+      <c r="F3200" t="n">
+        <v>8.199999999999999</v>
+      </c>
+      <c r="G3200" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3200" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3201" spans="1:8">
       <c r="A3201" s="1" t="n">
@@ -87685,12 +89365,24 @@
       <c r="B3201" t="s">
         <v>194</v>
       </c>
-      <c r="C3201" t="s"/>
-      <c r="D3201" t="s"/>
-      <c r="E3201" t="s"/>
-      <c r="F3201" t="s"/>
-      <c r="G3201" t="s"/>
-      <c r="H3201" t="s"/>
+      <c r="C3201" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="D3201" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3201" t="n">
+        <v>80.90000000000001</v>
+      </c>
+      <c r="F3201" t="n">
+        <v>91.2</v>
+      </c>
+      <c r="G3201" t="n">
+        <v>70.09999999999999</v>
+      </c>
+      <c r="H3201" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3202" spans="1:8">
       <c r="A3202" s="1" t="n">
@@ -87699,12 +89391,24 @@
       <c r="B3202" t="s">
         <v>194</v>
       </c>
-      <c r="C3202" t="s"/>
-      <c r="D3202" t="s"/>
-      <c r="E3202" t="s"/>
-      <c r="F3202" t="s"/>
-      <c r="G3202" t="s"/>
-      <c r="H3202" t="s"/>
+      <c r="C3202" t="n">
+        <v>4</v>
+      </c>
+      <c r="D3202" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3202" t="n">
+        <v>83.8</v>
+      </c>
+      <c r="F3202" t="n">
+        <v>77.59999999999999</v>
+      </c>
+      <c r="G3202" t="n">
+        <v>111.7</v>
+      </c>
+      <c r="H3202" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3203" spans="1:8">
       <c r="A3203" s="1" t="n">
@@ -87713,12 +89417,24 @@
       <c r="B3203" t="s">
         <v>195</v>
       </c>
-      <c r="C3203" t="s"/>
-      <c r="D3203" t="s"/>
-      <c r="E3203" t="s"/>
-      <c r="F3203" t="s"/>
-      <c r="G3203" t="s"/>
-      <c r="H3203" t="s"/>
+      <c r="C3203" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="D3203" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3203" t="n">
+        <v>69.5</v>
+      </c>
+      <c r="F3203" t="n">
+        <v>92.40000000000001</v>
+      </c>
+      <c r="G3203" t="n">
+        <v>64.7</v>
+      </c>
+      <c r="H3203" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3204" spans="1:8">
       <c r="A3204" s="1" t="n">
@@ -89703,12 +91419,24 @@
       <c r="B3280" t="s">
         <v>247</v>
       </c>
-      <c r="C3280" t="s"/>
-      <c r="D3280" t="s"/>
-      <c r="E3280" t="s"/>
-      <c r="F3280" t="s"/>
-      <c r="G3280" t="s"/>
-      <c r="H3280" t="s"/>
+      <c r="C3280" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="D3280" t="n">
+        <v>112.5</v>
+      </c>
+      <c r="E3280" t="n">
+        <v>92.59999999999999</v>
+      </c>
+      <c r="F3280" t="n">
+        <v>100.2</v>
+      </c>
+      <c r="G3280" t="n">
+        <v>71.8</v>
+      </c>
+      <c r="H3280" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3281" spans="1:8">
       <c r="A3281" s="1" t="n">
@@ -89717,12 +91445,24 @@
       <c r="B3281" t="s">
         <v>201</v>
       </c>
-      <c r="C3281" t="s"/>
-      <c r="D3281" t="s"/>
-      <c r="E3281" t="s"/>
-      <c r="F3281" t="s"/>
-      <c r="G3281" t="s"/>
-      <c r="H3281" t="s"/>
+      <c r="C3281" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="D3281" t="n">
+        <v>112.5</v>
+      </c>
+      <c r="E3281" t="n">
+        <v>103.4</v>
+      </c>
+      <c r="F3281" t="n">
+        <v>110.8</v>
+      </c>
+      <c r="G3281" t="n">
+        <v>88.3</v>
+      </c>
+      <c r="H3281" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3282" spans="1:8">
       <c r="A3282" s="1" t="n">
@@ -89731,12 +91471,24 @@
       <c r="B3282" t="s">
         <v>200</v>
       </c>
-      <c r="C3282" t="s"/>
-      <c r="D3282" t="s"/>
-      <c r="E3282" t="s"/>
-      <c r="F3282" t="s"/>
-      <c r="G3282" t="s"/>
-      <c r="H3282" t="s"/>
+      <c r="C3282" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="D3282" t="n">
+        <v>87.5</v>
+      </c>
+      <c r="E3282" t="n">
+        <v>89.59999999999999</v>
+      </c>
+      <c r="F3282" t="n">
+        <v>131.4</v>
+      </c>
+      <c r="G3282" t="n">
+        <v>73.40000000000001</v>
+      </c>
+      <c r="H3282" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3283" spans="1:8">
       <c r="A3283" s="1" t="n">
@@ -91253,12 +93005,24 @@
       <c r="B3341" t="s">
         <v>247</v>
       </c>
-      <c r="C3341" t="s"/>
-      <c r="D3341" t="s"/>
-      <c r="E3341" t="s"/>
-      <c r="F3341" t="s"/>
-      <c r="G3341" t="s"/>
-      <c r="H3341" t="s"/>
+      <c r="C3341" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="D3341" t="n">
+        <v>52.9</v>
+      </c>
+      <c r="E3341" t="n">
+        <v>67.7</v>
+      </c>
+      <c r="F3341" t="n">
+        <v>72.5</v>
+      </c>
+      <c r="G3341" t="n">
+        <v>77.5</v>
+      </c>
+      <c r="H3341" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3342" spans="1:8">
       <c r="A3342" s="1" t="n">
@@ -91267,12 +93031,24 @@
       <c r="B3342" t="s">
         <v>197</v>
       </c>
-      <c r="C3342" t="s"/>
-      <c r="D3342" t="s"/>
-      <c r="E3342" t="s"/>
-      <c r="F3342" t="s"/>
-      <c r="G3342" t="s"/>
-      <c r="H3342" t="s"/>
+      <c r="C3342" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3342" t="n">
+        <v>63.5</v>
+      </c>
+      <c r="E3342" t="n">
+        <v>55</v>
+      </c>
+      <c r="F3342" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="G3342" t="n">
+        <v>74.40000000000001</v>
+      </c>
+      <c r="H3342" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3343" spans="1:8">
       <c r="A3343" s="1" t="n">
@@ -91281,12 +93057,24 @@
       <c r="B3343" t="s">
         <v>200</v>
       </c>
-      <c r="C3343" t="s"/>
-      <c r="D3343" t="s"/>
-      <c r="E3343" t="s"/>
-      <c r="F3343" t="s"/>
-      <c r="G3343" t="s"/>
-      <c r="H3343" t="s"/>
+      <c r="C3343" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="D3343" t="n">
+        <v>58.2</v>
+      </c>
+      <c r="E3343" t="n">
+        <v>63.5</v>
+      </c>
+      <c r="F3343" t="n">
+        <v>50</v>
+      </c>
+      <c r="G3343" t="n">
+        <v>72.40000000000001</v>
+      </c>
+      <c r="H3343" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3344" spans="1:8">
       <c r="A3344" s="1" t="n">
@@ -91295,12 +93083,24 @@
       <c r="B3344" t="s">
         <v>247</v>
       </c>
-      <c r="C3344" t="s"/>
-      <c r="D3344" t="s"/>
-      <c r="E3344" t="s"/>
-      <c r="F3344" t="s"/>
-      <c r="G3344" t="s"/>
-      <c r="H3344" t="s"/>
+      <c r="C3344" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="D3344" t="n">
+        <v>63.5</v>
+      </c>
+      <c r="E3344" t="n">
+        <v>79</v>
+      </c>
+      <c r="F3344" t="n">
+        <v>63.8</v>
+      </c>
+      <c r="G3344" t="n">
+        <v>80.2</v>
+      </c>
+      <c r="H3344" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3345" spans="1:8">
       <c r="A3345" s="1" t="n">
@@ -91309,12 +93109,24 @@
       <c r="B3345" t="s">
         <v>195</v>
       </c>
-      <c r="C3345" t="s"/>
-      <c r="D3345" t="s"/>
-      <c r="E3345" t="s"/>
-      <c r="F3345" t="s"/>
-      <c r="G3345" t="s"/>
-      <c r="H3345" t="s"/>
+      <c r="C3345" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="D3345" t="n">
+        <v>74.09999999999999</v>
+      </c>
+      <c r="E3345" t="n">
+        <v>83.40000000000001</v>
+      </c>
+      <c r="F3345" t="n">
+        <v>63.5</v>
+      </c>
+      <c r="G3345" t="n">
+        <v>89.8</v>
+      </c>
+      <c r="H3345" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3346" spans="1:8">
       <c r="A3346" s="1" t="n">
@@ -91323,12 +93135,24 @@
       <c r="B3346" t="s">
         <v>201</v>
       </c>
-      <c r="C3346" t="s"/>
-      <c r="D3346" t="s"/>
-      <c r="E3346" t="s"/>
-      <c r="F3346" t="s"/>
-      <c r="G3346" t="s"/>
-      <c r="H3346" t="s"/>
+      <c r="C3346" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="D3346" t="n">
+        <v>68.8</v>
+      </c>
+      <c r="E3346" t="n">
+        <v>97.40000000000001</v>
+      </c>
+      <c r="F3346" t="n">
+        <v>85.09999999999999</v>
+      </c>
+      <c r="G3346" t="n">
+        <v>118.8</v>
+      </c>
+      <c r="H3346" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3347" spans="1:8">
       <c r="A3347" s="1" t="n">
@@ -91337,12 +93161,24 @@
       <c r="B3347" t="s">
         <v>201</v>
       </c>
-      <c r="C3347" t="s"/>
-      <c r="D3347" t="s"/>
-      <c r="E3347" t="s"/>
-      <c r="F3347" t="s"/>
-      <c r="G3347" t="s"/>
-      <c r="H3347" t="s"/>
+      <c r="C3347" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="D3347" t="n">
+        <v>52.9</v>
+      </c>
+      <c r="E3347" t="n">
+        <v>73.5</v>
+      </c>
+      <c r="F3347" t="n">
+        <v>75.2</v>
+      </c>
+      <c r="G3347" t="n">
+        <v>59.6</v>
+      </c>
+      <c r="H3347" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3348" spans="1:8">
       <c r="A3348" s="1" t="n">
@@ -91351,12 +93187,24 @@
       <c r="B3348" t="s">
         <v>200</v>
       </c>
-      <c r="C3348" t="s"/>
-      <c r="D3348" t="s"/>
-      <c r="E3348" t="s"/>
-      <c r="F3348" t="s"/>
-      <c r="G3348" t="s"/>
-      <c r="H3348" t="s"/>
+      <c r="C3348" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="D3348" t="n">
+        <v>63.5</v>
+      </c>
+      <c r="E3348" t="n">
+        <v>66</v>
+      </c>
+      <c r="F3348" t="n">
+        <v>53.5</v>
+      </c>
+      <c r="G3348" t="n">
+        <v>64.7</v>
+      </c>
+      <c r="H3348" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3349" spans="1:8">
       <c r="A3349" s="1" t="n">
@@ -91365,12 +93213,24 @@
       <c r="B3349" t="s">
         <v>200</v>
       </c>
-      <c r="C3349" t="s"/>
-      <c r="D3349" t="s"/>
-      <c r="E3349" t="s"/>
-      <c r="F3349" t="s"/>
-      <c r="G3349" t="s"/>
-      <c r="H3349" t="s"/>
+      <c r="C3349" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="D3349" t="n">
+        <v>52.9</v>
+      </c>
+      <c r="E3349" t="n">
+        <v>60.2</v>
+      </c>
+      <c r="F3349" t="n">
+        <v>38.7</v>
+      </c>
+      <c r="G3349" t="n">
+        <v>94.40000000000001</v>
+      </c>
+      <c r="H3349" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3350" spans="1:8">
       <c r="A3350" s="1" t="n">
@@ -91379,12 +93239,24 @@
       <c r="B3350" t="s">
         <v>195</v>
       </c>
-      <c r="C3350" t="s"/>
-      <c r="D3350" t="s"/>
-      <c r="E3350" t="s"/>
-      <c r="F3350" t="s"/>
-      <c r="G3350" t="s"/>
-      <c r="H3350" t="s"/>
+      <c r="C3350" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="D3350" t="n">
+        <v>52.9</v>
+      </c>
+      <c r="E3350" t="n">
+        <v>99.2</v>
+      </c>
+      <c r="F3350" t="n">
+        <v>75.5</v>
+      </c>
+      <c r="G3350" t="n">
+        <v>95.3</v>
+      </c>
+      <c r="H3350" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3351" spans="1:8">
       <c r="A3351" s="1" t="n">
@@ -91393,12 +93265,24 @@
       <c r="B3351" t="s">
         <v>201</v>
       </c>
-      <c r="C3351" t="s"/>
-      <c r="D3351" t="s"/>
-      <c r="E3351" t="s"/>
-      <c r="F3351" t="s"/>
-      <c r="G3351" t="s"/>
-      <c r="H3351" t="s"/>
+      <c r="C3351" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3351" t="n">
+        <v>52.9</v>
+      </c>
+      <c r="E3351" t="n">
+        <v>65.59999999999999</v>
+      </c>
+      <c r="F3351" t="n">
+        <v>58.3</v>
+      </c>
+      <c r="G3351" t="n">
+        <v>63.8</v>
+      </c>
+      <c r="H3351" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3352" spans="1:8">
       <c r="A3352" s="1" t="n">
@@ -91407,12 +93291,24 @@
       <c r="B3352" t="s">
         <v>200</v>
       </c>
-      <c r="C3352" t="s"/>
-      <c r="D3352" t="s"/>
-      <c r="E3352" t="s"/>
-      <c r="F3352" t="s"/>
-      <c r="G3352" t="s"/>
-      <c r="H3352" t="s"/>
+      <c r="C3352" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="D3352" t="n">
+        <v>52.9</v>
+      </c>
+      <c r="E3352" t="n">
+        <v>92.7</v>
+      </c>
+      <c r="F3352" t="n">
+        <v>67.90000000000001</v>
+      </c>
+      <c r="G3352" t="n">
+        <v>139.1</v>
+      </c>
+      <c r="H3352" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3353" spans="1:8">
       <c r="A3353" s="1" t="n">
@@ -91421,12 +93317,24 @@
       <c r="B3353" t="s">
         <v>247</v>
       </c>
-      <c r="C3353" t="s"/>
-      <c r="D3353" t="s"/>
-      <c r="E3353" t="s"/>
-      <c r="F3353" t="s"/>
-      <c r="G3353" t="s"/>
-      <c r="H3353" t="s"/>
+      <c r="C3353" t="n">
+        <v>4</v>
+      </c>
+      <c r="D3353" t="n">
+        <v>63.5</v>
+      </c>
+      <c r="E3353" t="n">
+        <v>85.90000000000001</v>
+      </c>
+      <c r="F3353" t="n">
+        <v>97.7</v>
+      </c>
+      <c r="G3353" t="n">
+        <v>70</v>
+      </c>
+      <c r="H3353" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3354" spans="1:8">
       <c r="A3354" s="1" t="n">
@@ -91435,12 +93343,24 @@
       <c r="B3354" t="s">
         <v>247</v>
       </c>
-      <c r="C3354" t="s"/>
-      <c r="D3354" t="s"/>
-      <c r="E3354" t="s"/>
-      <c r="F3354" t="s"/>
-      <c r="G3354" t="s"/>
-      <c r="H3354" t="s"/>
+      <c r="C3354" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="D3354" t="n">
+        <v>39</v>
+      </c>
+      <c r="E3354" t="n">
+        <v>59.7</v>
+      </c>
+      <c r="F3354" t="n">
+        <v>63.2</v>
+      </c>
+      <c r="G3354" t="n">
+        <v>55.9</v>
+      </c>
+      <c r="H3354" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3355" spans="1:8">
       <c r="A3355" s="1" t="n">

</xml_diff>